<commit_message>
Some other typos fixed #1
</commit_message>
<xml_diff>
--- a/VSCode/Blocking Deletion of Warehouse Shipment Lines/Test/atdd.scenarios/ATDD Scenarios - Blocking Deletion of Warehouse Shipment Lines.xlsx
+++ b/VSCode/Blocking Deletion of Warehouse Shipment Lines/Test/atdd.scenarios/ATDD Scenarios - Blocking Deletion of Warehouse Shipment Lines.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc van Vugt\OneDrive\Training\Test Automation\Online Crash Course - March 2020\Business Case - Blocking Deletion of Warehouse Shipment Lines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc van Vugt\source\repos\Test-Automation-Examples\VSCode\Blocking Deletion of Warehouse Shipment Lines\Test\atdd.scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="352" documentId="13_ncr:1_{6A470D69-49E4-4B9E-87A1-2100173A9F5F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{9D4C3EF8-2145-469A-A68B-7C11864C3626}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8751918-6E3E-4045-90EF-D2382E390DBC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28050" windowHeight="16440" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
   </bookViews>
@@ -99,93 +99,6 @@
     <t>Warehouse employee for current user with allowance</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Delete by user with </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>no</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> allowance automatically created whse shpt. line</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Delete by user with </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>no</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> allowance manually created whse shpt. line</t>
-    </r>
-  </si>
-  <si>
-    <t>Delete by user with allowance manually created whse shpt. line</t>
-  </si>
-  <si>
-    <t>Delete by user with allowance automatically created whse shpt. line</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Delete  by user with </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>no</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> allowance manually created whse shpt. line</t>
-    </r>
-  </si>
-  <si>
     <t>Allowed to Delete Shpt. Line is hidden on warehouse employee card</t>
   </si>
   <si>
@@ -207,36 +120,6 @@
     <t>Delete warehouse shipment line and select yes in confirm</t>
   </si>
   <si>
-    <t>Delete  by user with allowance automatically created whse shpt. Line with confirmation</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Delete  by user with allowance automatically created whse shpt. Line with </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">no </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>confirmation</t>
-    </r>
-  </si>
-  <si>
     <t>Delete warehouse shipment line and select no in confirm</t>
   </si>
   <si>
@@ -250,6 +133,27 @@
   </si>
   <si>
     <t>Disable "Unblock Deletion of Shpt. Line" on warehouse setup</t>
+  </si>
+  <si>
+    <t>Delete by user with no allowance manually created whse. shpt. line</t>
+  </si>
+  <si>
+    <t>Delete by user with no allowance automatically created whse. shpt. line</t>
+  </si>
+  <si>
+    <t>Delete by user with allowance manually created whse. shpt. line</t>
+  </si>
+  <si>
+    <t>Delete by user with allowance automatically created whse. shpt. line</t>
+  </si>
+  <si>
+    <t>Delete  by user with no allowance manually created whse. shpt. line</t>
+  </si>
+  <si>
+    <t>Delete  by user with allowance automatically created whse. shpt. line with confirmation</t>
+  </si>
+  <si>
+    <t>Delete  by user with allowance automatically created whse. shpt. line with no confirmation</t>
   </si>
 </sst>
 </file>
@@ -259,7 +163,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,15 +176,6 @@
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -338,7 +233,55 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="18">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -400,256 +343,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -664,24 +357,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:K74" totalsRowShown="0" headerRowDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:K74" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A1:K74" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{8363E7FF-10AC-4A2B-AF58-2B6F4A3A2982}" name="Feature" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{47ED26B9-CBC1-4AA1-A3A9-843BF13AA89B}" name="Sub Feature" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="31"/>
-    <tableColumn id="11" xr3:uid="{FC90C2DF-011C-4E76-8C03-6E75B2478287}" name="Positive-negative" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{8363E7FF-10AC-4A2B-AF58-2B6F4A3A2982}" name="Feature" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{47ED26B9-CBC1-4AA1-A3A9-843BF13AA89B}" name="Sub Feature" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{FC90C2DF-011C-4E76-8C03-6E75B2478287}" name="Positive-negative" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{824F4994-529B-42E7-960A-C52362C8177D}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="33">
+    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="2">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="37">
+    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -986,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B1ED69-5F96-4A81-993F-0E906F475813}">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +709,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1042,7 +735,7 @@
     </row>
     <row r="2" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -1058,28 +751,28 @@
     </row>
     <row r="3" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="H3" s="5">
         <v>1</v>
       </c>
       <c r="I3" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0001] Delete by user with no allowance manually created whse shpt. line</v>
+        <v>[SCENARIO #0001] Delete by user with no allowance manually created whse. shpt. line</v>
       </c>
       <c r="J3" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0001] Delete by user with no allowance manually created whse shpt. line</v>
+        <v>//[SCENARIO #0001] Delete by user with no allowance manually created whse. shpt. line</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -1087,7 +780,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H4" s="5">
         <v>1</v>
@@ -1103,7 +796,7 @@
     </row>
     <row r="5" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -1127,7 +820,7 @@
     </row>
     <row r="6" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -1151,7 +844,7 @@
     </row>
     <row r="7" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -1175,7 +868,7 @@
     </row>
     <row r="8" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -1199,7 +892,7 @@
     </row>
     <row r="9" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -1223,28 +916,28 @@
     </row>
     <row r="10" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="3" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="H10" s="5">
         <v>2</v>
       </c>
       <c r="I10" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0002] Delete by user with no allowance automatically created whse shpt. line</v>
+        <v>[SCENARIO #0002] Delete by user with no allowance automatically created whse. shpt. line</v>
       </c>
       <c r="J10" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0002] Delete by user with no allowance automatically created whse shpt. line</v>
+        <v>//[SCENARIO #0002] Delete by user with no allowance automatically created whse. shpt. line</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -1252,7 +945,7 @@
         <v>10</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H11" s="5">
         <v>2</v>
@@ -1268,7 +961,7 @@
     </row>
     <row r="12" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -1292,7 +985,7 @@
     </row>
     <row r="13" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -1316,7 +1009,7 @@
     </row>
     <row r="14" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -1340,7 +1033,7 @@
     </row>
     <row r="15" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -1364,7 +1057,7 @@
     </row>
     <row r="16" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -1388,28 +1081,28 @@
     </row>
     <row r="17" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="3" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="H17" s="5">
         <v>3</v>
       </c>
       <c r="I17" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0003] Delete by user with allowance manually created whse shpt. line</v>
+        <v>[SCENARIO #0003] Delete by user with allowance manually created whse. shpt. line</v>
       </c>
       <c r="J17" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0003] Delete by user with allowance manually created whse shpt. line</v>
+        <v>//[SCENARIO #0003] Delete by user with allowance manually created whse. shpt. line</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -1417,7 +1110,7 @@
         <v>10</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H18" s="5">
         <v>3</v>
@@ -1433,7 +1126,7 @@
     </row>
     <row r="19" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -1457,7 +1150,7 @@
     </row>
     <row r="20" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -1481,7 +1174,7 @@
     </row>
     <row r="21" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -1505,7 +1198,7 @@
     </row>
     <row r="22" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -1529,7 +1222,7 @@
     </row>
     <row r="23" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -1553,28 +1246,28 @@
     </row>
     <row r="24" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="H24" s="5">
         <v>4</v>
       </c>
       <c r="I24" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0004] Delete by user with allowance automatically created whse shpt. line</v>
+        <v>[SCENARIO #0004] Delete by user with allowance automatically created whse. shpt. line</v>
       </c>
       <c r="J24" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0004] Delete by user with allowance automatically created whse shpt. line</v>
+        <v>//[SCENARIO #0004] Delete by user with allowance automatically created whse. shpt. line</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -1582,7 +1275,7 @@
         <v>10</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H25" s="5">
         <v>4</v>
@@ -1598,7 +1291,7 @@
     </row>
     <row r="26" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -1622,7 +1315,7 @@
     </row>
     <row r="27" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -1646,7 +1339,7 @@
     </row>
     <row r="28" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -1670,7 +1363,7 @@
     </row>
     <row r="29" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -1694,7 +1387,7 @@
     </row>
     <row r="30" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -1718,14 +1411,14 @@
     </row>
     <row r="31" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="H31" s="5">
         <v>9</v>
@@ -1741,7 +1434,7 @@
     </row>
     <row r="32" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>13</v>
@@ -1767,7 +1460,7 @@
     </row>
     <row r="33" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>13</v>
@@ -1777,7 +1470,7 @@
         <v>11</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H33" s="5">
         <v>9</v>
@@ -1793,7 +1486,7 @@
     </row>
     <row r="34" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>13</v>
@@ -1803,7 +1496,7 @@
         <v>12</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H34" s="5">
         <v>9</v>
@@ -1819,7 +1512,7 @@
     </row>
     <row r="35" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -1834,28 +1527,28 @@
     </row>
     <row r="36" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
       <c r="E36" s="3" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="H36" s="5">
         <v>5</v>
       </c>
       <c r="I36" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0005] Delete  by user with no allowance manually created whse shpt. line</v>
+        <v>[SCENARIO #0005] Delete  by user with no allowance manually created whse. shpt. line</v>
       </c>
       <c r="J36" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0005] Delete  by user with no allowance manually created whse shpt. line</v>
+        <v>//[SCENARIO #0005] Delete  by user with no allowance manually created whse. shpt. line</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
@@ -1863,7 +1556,7 @@
         <v>10</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H37" s="5">
         <v>5</v>
@@ -1879,7 +1572,7 @@
     </row>
     <row r="38" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
@@ -1903,7 +1596,7 @@
     </row>
     <row r="39" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -1927,7 +1620,7 @@
     </row>
     <row r="40" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
@@ -1951,7 +1644,7 @@
     </row>
     <row r="41" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
@@ -1975,7 +1668,7 @@
     </row>
     <row r="42" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
@@ -1999,30 +1692,30 @@
     </row>
     <row r="43" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="H43" s="5">
         <v>6</v>
       </c>
       <c r="I43" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0006] Delete by user with no allowance automatically created whse shpt. line</v>
+        <v>[SCENARIO #0006] Delete by user with no allowance automatically created whse. shpt. line</v>
       </c>
       <c r="J43" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0006] Delete by user with no allowance automatically created whse shpt. line</v>
+        <v>//[SCENARIO #0006] Delete by user with no allowance automatically created whse. shpt. line</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="10" t="s">
@@ -2032,7 +1725,7 @@
         <v>10</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H44" s="5">
         <v>6</v>
@@ -2048,7 +1741,7 @@
     </row>
     <row r="45" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="10" t="s">
@@ -2074,7 +1767,7 @@
     </row>
     <row r="46" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="10" t="s">
@@ -2100,7 +1793,7 @@
     </row>
     <row r="47" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="10" t="s">
@@ -2126,7 +1819,7 @@
     </row>
     <row r="48" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="10" t="s">
@@ -2152,7 +1845,7 @@
     </row>
     <row r="49" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10" t="s">
@@ -2162,7 +1855,7 @@
         <v>12</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H49" s="5">
         <v>6</v>
@@ -2178,28 +1871,28 @@
     </row>
     <row r="50" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
       <c r="E50" s="3" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="H50" s="5">
         <v>7</v>
       </c>
       <c r="I50" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0007] Delete by user with allowance manually created whse shpt. line</v>
+        <v>[SCENARIO #0007] Delete by user with allowance manually created whse. shpt. line</v>
       </c>
       <c r="J50" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0007] Delete by user with allowance manually created whse shpt. line</v>
+        <v>//[SCENARIO #0007] Delete by user with allowance manually created whse. shpt. line</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
@@ -2207,7 +1900,7 @@
         <v>10</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H51" s="5">
         <v>7</v>
@@ -2223,7 +1916,7 @@
     </row>
     <row r="52" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
@@ -2247,7 +1940,7 @@
     </row>
     <row r="53" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
@@ -2271,7 +1964,7 @@
     </row>
     <row r="54" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
@@ -2295,7 +1988,7 @@
     </row>
     <row r="55" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
@@ -2319,7 +2012,7 @@
     </row>
     <row r="56" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
@@ -2343,28 +2036,28 @@
     </row>
     <row r="57" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
       <c r="E57" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="H57" s="5">
         <v>8</v>
       </c>
       <c r="I57" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0008] Delete  by user with allowance automatically created whse shpt. Line with confirmation</v>
+        <v>[SCENARIO #0008] Delete  by user with allowance automatically created whse. shpt. line with confirmation</v>
       </c>
       <c r="J57" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0008] Delete  by user with allowance automatically created whse shpt. Line with confirmation</v>
+        <v>//[SCENARIO #0008] Delete  by user with allowance automatically created whse. shpt. line with confirmation</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
@@ -2372,7 +2065,7 @@
         <v>10</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H58" s="5">
         <v>8</v>
@@ -2388,7 +2081,7 @@
     </row>
     <row r="59" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
@@ -2412,7 +2105,7 @@
     </row>
     <row r="60" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
@@ -2436,7 +2129,7 @@
     </row>
     <row r="61" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
@@ -2460,7 +2153,7 @@
     </row>
     <row r="62" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
@@ -2468,7 +2161,7 @@
         <v>11</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H62" s="5">
         <v>8</v>
@@ -2484,7 +2177,7 @@
     </row>
     <row r="63" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
@@ -2508,30 +2201,30 @@
     </row>
     <row r="64" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C64" s="10"/>
       <c r="D64" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H64" s="5">
         <v>11</v>
       </c>
       <c r="I64" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0011] Delete  by user with allowance automatically created whse shpt. Line with no confirmation</v>
+        <v>[SCENARIO #0011] Delete  by user with allowance automatically created whse. shpt. line with no confirmation</v>
       </c>
       <c r="J64" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0011] Delete  by user with allowance automatically created whse shpt. Line with no confirmation</v>
+        <v>//[SCENARIO #0011] Delete  by user with allowance automatically created whse. shpt. line with no confirmation</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C65" s="10"/>
       <c r="D65" s="10" t="s">
@@ -2541,7 +2234,7 @@
         <v>10</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H65" s="5">
         <v>11</v>
@@ -2557,7 +2250,7 @@
     </row>
     <row r="66" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C66" s="10"/>
       <c r="D66" s="10" t="s">
@@ -2583,7 +2276,7 @@
     </row>
     <row r="67" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C67" s="10"/>
       <c r="D67" s="10" t="s">
@@ -2609,7 +2302,7 @@
     </row>
     <row r="68" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C68" s="10"/>
       <c r="D68" s="10" t="s">
@@ -2635,7 +2328,7 @@
     </row>
     <row r="69" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C69" s="10"/>
       <c r="D69" s="10" t="s">
@@ -2645,7 +2338,7 @@
         <v>11</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="H69" s="5">
         <v>11</v>
@@ -2661,7 +2354,7 @@
     </row>
     <row r="70" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C70" s="10"/>
       <c r="D70" s="10" t="s">
@@ -2671,7 +2364,7 @@
         <v>12</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H70" s="5">
         <v>11</v>
@@ -2687,14 +2380,14 @@
     </row>
     <row r="71" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C71" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D71" s="10"/>
       <c r="E71" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H71" s="5">
         <v>10</v>
@@ -2710,7 +2403,7 @@
     </row>
     <row r="72" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>13</v>
@@ -2736,7 +2429,7 @@
     </row>
     <row r="73" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C73" s="10" t="s">
         <v>13</v>
@@ -2746,7 +2439,7 @@
         <v>11</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H73" s="5">
         <v>10</v>
@@ -2762,7 +2455,7 @@
     </row>
     <row r="74" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C74" s="10" t="s">
         <v>13</v>
@@ -2772,7 +2465,7 @@
         <v>12</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H74" s="5">
         <v>10</v>
@@ -2800,31 +2493,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="disabled">
+    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="disabled">
       <formula>NOT(ISERROR(SEARCH("disabled",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="enabled">
+    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="enabled">
       <formula>NOT(ISERROR(SEARCH("enabled",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated ATDD scenarios and test case implemntation accordingly #1
</commit_message>
<xml_diff>
--- a/VSCode/Blocking Deletion of Warehouse Shipment Lines/Test/atdd.scenarios/ATDD Scenarios - Blocking Deletion of Warehouse Shipment Lines.xlsx
+++ b/VSCode/Blocking Deletion of Warehouse Shipment Lines/Test/atdd.scenarios/ATDD Scenarios - Blocking Deletion of Warehouse Shipment Lines.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc van Vugt\source\repos\Test-Automation-Examples\VSCode\Blocking Deletion of Warehouse Shipment Lines\Test\atdd.scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc van Vugt\OneDrive\Training\Test Automation\Online Crash Course - March 2020\Business Case - Blocking Deletion of Warehouse Shipment Lines\Code\VSCode\Test\atdd.scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8751918-6E3E-4045-90EF-D2382E390DBC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{F8751918-6E3E-4045-90EF-D2382E390DBC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{8F113CA0-FAF8-4005-954D-A91E43D44866}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28050" windowHeight="16440" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="43">
   <si>
     <t>Feature</t>
   </si>
@@ -99,18 +99,6 @@
     <t>Warehouse employee for current user with allowance</t>
   </si>
   <si>
-    <t>Allowed to Delete Shpt. Line is hidden on warehouse employee card</t>
-  </si>
-  <si>
-    <t>Allowed to Delete Shpt. Line is hidden</t>
-  </si>
-  <si>
-    <t>Allowed to Delete Shpt. Line is visible</t>
-  </si>
-  <si>
-    <t>Allowed to Delete Shpt. Line is visible on warehouse employee card</t>
-  </si>
-  <si>
     <t>Positive-negative</t>
   </si>
   <si>
@@ -144,16 +132,34 @@
     <t>Delete by user with allowance manually created whse. shpt. line</t>
   </si>
   <si>
-    <t>Delete by user with allowance automatically created whse. shpt. line</t>
-  </si>
-  <si>
     <t>Delete  by user with no allowance manually created whse. shpt. line</t>
   </si>
   <si>
     <t>Delete  by user with allowance automatically created whse. shpt. line with confirmation</t>
   </si>
   <si>
-    <t>Delete  by user with allowance automatically created whse. shpt. line with no confirmation</t>
+    <t>Allowed to Delete Shpt. Line is editable on warehouse employees page</t>
+  </si>
+  <si>
+    <t>Allowed to Delete Shpt. Line is not editable on warehouse employees page</t>
+  </si>
+  <si>
+    <t>"Allowed to Delete Shpt. Line" is not editable on warehouse employees page</t>
+  </si>
+  <si>
+    <t>"Allowed to Delete Shpt. Line" is editable on warehouse employees page</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Delete by user with allowance automatically created whse. shpt. line with no confirmation</t>
+  </si>
+  <si>
+    <t>Empty error occurred</t>
+  </si>
+  <si>
+    <t>Delete  by user with allowance automatically created whse. shpt. Line</t>
   </si>
 </sst>
 </file>
@@ -233,7 +239,99 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -282,67 +380,6 @@
     <dxf>
       <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -357,24 +394,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:K74" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A1:K74" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:K76" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A1:K76" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{8363E7FF-10AC-4A2B-AF58-2B6F4A3A2982}" name="Feature" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{47ED26B9-CBC1-4AA1-A3A9-843BF13AA89B}" name="Sub Feature" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{FC90C2DF-011C-4E76-8C03-6E75B2478287}" name="Positive-negative" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{8363E7FF-10AC-4A2B-AF58-2B6F4A3A2982}" name="Feature" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{47ED26B9-CBC1-4AA1-A3A9-843BF13AA89B}" name="Sub Feature" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{FC90C2DF-011C-4E76-8C03-6E75B2478287}" name="Positive-negative" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="16"/>
     <tableColumn id="3" xr3:uid="{824F4994-529B-42E7-960A-C52362C8177D}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="13">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="1">
+    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="12">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -677,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B1ED69-5F96-4A81-993F-0E906F475813}">
-  <dimension ref="A1:K74"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,7 +746,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -735,7 +772,7 @@
     </row>
     <row r="2" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -751,12 +788,12 @@
     </row>
     <row r="3" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H3" s="5">
         <v>1</v>
@@ -772,7 +809,7 @@
     </row>
     <row r="4" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -780,7 +817,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H4" s="5">
         <v>1</v>
@@ -796,7 +833,7 @@
     </row>
     <row r="5" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -820,7 +857,7 @@
     </row>
     <row r="6" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -844,7 +881,7 @@
     </row>
     <row r="7" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -868,7 +905,7 @@
     </row>
     <row r="8" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -892,7 +929,7 @@
     </row>
     <row r="9" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -916,12 +953,14 @@
     </row>
     <row r="10" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="D10" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="E10" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H10" s="5">
         <v>2</v>
@@ -937,15 +976,17 @@
     </row>
     <row r="11" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
+      <c r="D11" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F11" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H11" s="5">
         <v>2</v>
@@ -961,10 +1002,12 @@
     </row>
     <row r="12" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
+      <c r="D12" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F12" t="s">
         <v>10</v>
       </c>
@@ -985,10 +1028,12 @@
     </row>
     <row r="13" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
+      <c r="D13" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F13" t="s">
         <v>10</v>
       </c>
@@ -1009,10 +1054,12 @@
     </row>
     <row r="14" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F14" t="s">
         <v>10</v>
       </c>
@@ -1033,10 +1080,12 @@
     </row>
     <row r="15" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
+      <c r="D15" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F15" t="s">
         <v>11</v>
       </c>
@@ -1057,36 +1106,38 @@
     </row>
     <row r="16" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
+      <c r="D16" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F16" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H16" s="5">
         <v>2</v>
       </c>
       <c r="I16" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Warehouse shipment line is deleted</v>
+        <v>[THEN] Error disallowing deletion</v>
       </c>
       <c r="J16" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Warehouse shipment line is deleted</v>
+        <v>//[THEN] Error disallowing deletion</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H17" s="5">
         <v>3</v>
@@ -1102,7 +1153,7 @@
     </row>
     <row r="18" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -1110,7 +1161,7 @@
         <v>10</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H18" s="5">
         <v>3</v>
@@ -1126,7 +1177,7 @@
     </row>
     <row r="19" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -1150,7 +1201,7 @@
     </row>
     <row r="20" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -1158,23 +1209,23 @@
         <v>10</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H20" s="5">
         <v>3</v>
       </c>
       <c r="I20" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user with no allowance</v>
+        <v>[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
       <c r="J20" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
+        <v>//[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -1198,7 +1249,7 @@
     </row>
     <row r="22" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -1222,7 +1273,7 @@
     </row>
     <row r="23" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -1246,28 +1297,28 @@
     </row>
     <row r="24" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H24" s="5">
         <v>4</v>
       </c>
       <c r="I24" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0004] Delete by user with allowance automatically created whse. shpt. line</v>
+        <v>[SCENARIO #0004] Delete  by user with allowance automatically created whse. shpt. line with confirmation</v>
       </c>
       <c r="J24" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0004] Delete by user with allowance automatically created whse. shpt. line</v>
+        <v>//[SCENARIO #0004] Delete  by user with allowance automatically created whse. shpt. line with confirmation</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -1275,7 +1326,7 @@
         <v>10</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H25" s="5">
         <v>4</v>
@@ -1291,7 +1342,7 @@
     </row>
     <row r="26" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -1315,7 +1366,7 @@
     </row>
     <row r="27" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -1339,7 +1390,7 @@
     </row>
     <row r="28" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -1363,7 +1414,7 @@
     </row>
     <row r="29" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -1371,23 +1422,23 @@
         <v>11</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H29" s="5">
         <v>4</v>
       </c>
       <c r="I29" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Delete warehouse shipment line</v>
+        <v>[WHEN] Delete warehouse shipment line and select yes in confirm</v>
       </c>
       <c r="J29" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Delete warehouse shipment line</v>
+        <v>//[WHEN] Delete warehouse shipment line and select yes in confirm</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -1411,677 +1462,693 @@
     </row>
     <row r="31" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="E31" s="3" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="H31" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I31" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0009] Allowed to Delete Shpt. Line is hidden</v>
+        <v>[SCENARIO #0011] Delete by user with allowance automatically created whse. shpt. line with no confirmation</v>
       </c>
       <c r="J31" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0009] Allowed to Delete Shpt. Line is hidden</v>
+        <v>//[SCENARIO #0011] Delete by user with allowance automatically created whse. shpt. line with no confirmation</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F32" t="s">
         <v>10</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="H32" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I32" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user</v>
+        <v>[GIVEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
       <c r="J32" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse employee for current user</v>
+        <v>//[GIVEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F33" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="5">
         <v>11</v>
       </c>
-      <c r="G33" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H33" s="5">
-        <v>9</v>
-      </c>
       <c r="I33" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+        <v>[GIVEN] Location with require shipment</v>
       </c>
       <c r="J33" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+        <v>//[GIVEN] Location with require shipment</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="5">
+        <v>11</v>
+      </c>
+      <c r="I34" s="6" t="str">
+        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Warehouse employee for current user with no allowance</v>
+      </c>
+      <c r="J34" s="7" t="str">
+        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35" s="5">
+        <v>11</v>
+      </c>
+      <c r="I35" s="6" t="str">
+        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
+      </c>
+      <c r="J35" s="7" t="str">
+        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H36" s="5">
+        <v>11</v>
+      </c>
+      <c r="I36" s="6" t="str">
+        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Delete warehouse shipment line and select no in confirm</v>
+      </c>
+      <c r="J36" s="7" t="str">
+        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Delete warehouse shipment line and select no in confirm</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" t="s">
         <v>12</v>
       </c>
-      <c r="G34" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H34" s="5">
+      <c r="G37" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H37" s="5">
+        <v>11</v>
+      </c>
+      <c r="I37" s="6" t="str">
+        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Empty error occurred</v>
+      </c>
+      <c r="J37" s="7" t="str">
+        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Empty error occurred</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="10"/>
+      <c r="E38" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H38" s="5">
         <v>9</v>
       </c>
-      <c r="I34" s="6" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Allowed to Delete Shpt. Line is hidden on warehouse employee card</v>
-      </c>
-      <c r="J34" s="7" t="str">
-        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Allowed to Delete Shpt. Line is hidden on warehouse employee card</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="I35" s="6" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[FEATURE] Unblock Deletion of Whse. Shpt. Line disabled/</v>
-      </c>
-      <c r="J35" s="7" t="str">
-        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[FEATURE] Unblock Deletion of Whse. Shpt. Line disabled/</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H36" s="5">
-        <v>5</v>
-      </c>
-      <c r="I36" s="6" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0005] Delete  by user with no allowance manually created whse. shpt. line</v>
-      </c>
-      <c r="J36" s="7" t="str">
-        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0005] Delete  by user with no allowance manually created whse. shpt. line</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="F37" t="s">
-        <v>10</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H37" s="5">
-        <v>5</v>
-      </c>
-      <c r="I37" s="6" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
-      </c>
-      <c r="J37" s="7" t="str">
-        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="F38" t="s">
-        <v>10</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H38" s="5">
-        <v>5</v>
-      </c>
       <c r="I38" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Location with require shipment</v>
+        <v>[SCENARIO #0009] "Allowed to Delete Shpt. Line" is editable on warehouse employees page</v>
       </c>
       <c r="J38" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Location with require shipment</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>//[SCENARIO #0009] "Allowed to Delete Shpt. Line" is editable on warehouse employees page</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="D39" s="10"/>
       <c r="F39" t="s">
         <v>10</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="H39" s="5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I39" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user with allowance</v>
+        <v>[GIVEN] Location</v>
       </c>
       <c r="J39" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse employee for current user with allowance</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>//[GIVEN] Location</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="D40" s="10"/>
       <c r="F40" t="s">
         <v>10</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H40" s="5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I40" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>[GIVEN] Warehouse employee for current user</v>
       </c>
       <c r="J40" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>//[GIVEN] Warehouse employee for current user</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="D41" s="10"/>
       <c r="F41" t="s">
         <v>11</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="H41" s="5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I41" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Delete warehouse shipment line</v>
+        <v>[WHEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
       <c r="J41" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Delete warehouse shipment line</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>//[WHEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C42" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="D42" s="10"/>
       <c r="F42" t="s">
         <v>12</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="H42" s="5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I42" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Warehouse shipment line is deleted</v>
+        <v>[THEN] Allowed to Delete Shpt. Line is editable on warehouse employees page</v>
       </c>
       <c r="J42" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Warehouse shipment line is deleted</v>
+        <v>//[THEN] Allowed to Delete Shpt. Line is editable on warehouse employees page</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C43" s="10"/>
-      <c r="D43" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H43" s="5">
-        <v>6</v>
-      </c>
+      <c r="D43" s="10"/>
       <c r="I43" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0006] Delete by user with no allowance automatically created whse. shpt. line</v>
+        <v>[FEATURE] Unblock Deletion of Whse. Shpt. Line disabled/</v>
       </c>
       <c r="J43" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0006] Delete by user with no allowance automatically created whse. shpt. line</v>
+        <v>//[FEATURE] Unblock Deletion of Whse. Shpt. Line disabled/</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C44" s="10"/>
-      <c r="D44" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G44" s="4" t="s">
+      <c r="D44" s="10"/>
+      <c r="E44" s="3" t="s">
         <v>33</v>
       </c>
       <c r="H44" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I44" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+        <v>[SCENARIO #0005] Delete  by user with no allowance manually created whse. shpt. line</v>
       </c>
       <c r="J44" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+        <v>//[SCENARIO #0005] Delete  by user with no allowance manually created whse. shpt. line</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C45" s="10"/>
-      <c r="D45" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D45" s="10"/>
       <c r="F45" t="s">
         <v>10</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="H45" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I45" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Location with require shipment</v>
+        <v>[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
       <c r="J45" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Location with require shipment</v>
+        <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C46" s="10"/>
-      <c r="D46" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D46" s="10"/>
       <c r="F46" t="s">
         <v>10</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H46" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I46" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user with no allowance</v>
+        <v>[GIVEN] Location with require shipment</v>
       </c>
       <c r="J46" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
+        <v>//[GIVEN] Location with require shipment</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C47" s="10"/>
-      <c r="D47" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D47" s="10"/>
       <c r="F47" t="s">
         <v>10</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H47" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I47" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
       <c r="J47" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>//[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C48" s="10"/>
-      <c r="D48" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D48" s="10"/>
       <c r="F48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H48" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I48" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Delete warehouse shipment line</v>
+        <v>[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
       <c r="J48" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Delete warehouse shipment line</v>
+        <v>//[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C49" s="10"/>
-      <c r="D49" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D49" s="10"/>
       <c r="F49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="H49" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I49" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Error disallowing deletion</v>
+        <v>[WHEN] Delete warehouse shipment line</v>
       </c>
       <c r="J49" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Error disallowing deletion</v>
+        <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
-      <c r="E50" s="3" t="s">
-        <v>36</v>
+      <c r="F50" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="H50" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I50" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0007] Delete by user with allowance manually created whse. shpt. line</v>
+        <v>[THEN] Warehouse shipment line is deleted</v>
       </c>
       <c r="J50" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0007] Delete by user with allowance manually created whse. shpt. line</v>
+        <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="F51" t="s">
-        <v>10</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="H51" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I51" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+        <v>[SCENARIO #0006] Delete by user with no allowance automatically created whse. shpt. line</v>
       </c>
       <c r="J51" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+        <v>//[SCENARIO #0006] Delete by user with no allowance automatically created whse. shpt. line</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
+      <c r="D52" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F52" t="s">
         <v>10</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="H52" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I52" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Location with require shipment</v>
+        <v>[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
       <c r="J52" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Location with require shipment</v>
+        <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
+      <c r="D53" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F53" t="s">
         <v>10</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H53" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I53" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user with allowance</v>
+        <v>[GIVEN] Location with require shipment</v>
       </c>
       <c r="J53" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse employee for current user with allowance</v>
+        <v>//[GIVEN] Location with require shipment</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
+      <c r="D54" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F54" t="s">
         <v>10</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H54" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I54" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
       <c r="J54" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
+      <c r="D55" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H55" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I55" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Delete warehouse shipment line</v>
+        <v>[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
       <c r="J55" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Delete warehouse shipment line</v>
+        <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
+      <c r="D56" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H56" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I56" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Warehouse shipment line is deleted</v>
+        <v>[WHEN] Delete warehouse shipment line</v>
       </c>
       <c r="J56" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Warehouse shipment line is deleted</v>
+        <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="3" t="s">
-        <v>39</v>
+      <c r="D57" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" t="s">
+        <v>12</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="H57" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I57" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0008] Delete  by user with allowance automatically created whse. shpt. line with confirmation</v>
+        <v>[THEN] Error disallowing deletion</v>
       </c>
       <c r="J57" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0008] Delete  by user with allowance automatically created whse. shpt. line with confirmation</v>
+        <v>//[THEN] Error disallowing deletion</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
-      <c r="F58" t="s">
-        <v>10</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>33</v>
+      <c r="E58" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="H58" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I58" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+        <v>[SCENARIO #0007] Delete by user with allowance manually created whse. shpt. line</v>
       </c>
       <c r="J58" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+        <v>//[SCENARIO #0007] Delete by user with allowance manually created whse. shpt. line</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
@@ -2089,23 +2156,23 @@
         <v>10</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="H59" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I59" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Location with require shipment</v>
+        <v>[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
       <c r="J59" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Location with require shipment</v>
+        <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
@@ -2113,23 +2180,23 @@
         <v>10</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H60" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I60" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user with no allowance</v>
+        <v>[GIVEN] Location with require shipment</v>
       </c>
       <c r="J60" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
+        <v>//[GIVEN] Location with require shipment</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
@@ -2137,120 +2204,118 @@
         <v>10</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H61" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I61" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
       <c r="J61" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>//[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
       <c r="F62" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="H62" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I62" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Delete warehouse shipment line and select yes in confirm</v>
+        <v>[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
       <c r="J62" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Delete warehouse shipment line and select yes in confirm</v>
+        <v>//[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
       <c r="F63" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H63" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I63" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Warehouse shipment line is deleted</v>
+        <v>[WHEN] Delete warehouse shipment line</v>
       </c>
       <c r="J63" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Warehouse shipment line is deleted</v>
+        <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C64" s="10"/>
-      <c r="D64" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>40</v>
+      <c r="D64" s="10"/>
+      <c r="F64" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="H64" s="5">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I64" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0011] Delete  by user with allowance automatically created whse. shpt. line with no confirmation</v>
+        <v>[THEN] Warehouse shipment line is deleted</v>
       </c>
       <c r="J64" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0011] Delete  by user with allowance automatically created whse. shpt. line with no confirmation</v>
+        <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C65" s="10"/>
       <c r="D65" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F65" t="s">
-        <v>10</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>33</v>
+      <c r="E65" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="H65" s="5">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I65" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+        <v>[SCENARIO #0008] Delete  by user with allowance automatically created whse. shpt. Line</v>
       </c>
       <c r="J65" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+        <v>//[SCENARIO #0008] Delete  by user with allowance automatically created whse. shpt. Line</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C66" s="10"/>
       <c r="D66" s="10" t="s">
@@ -2260,23 +2325,23 @@
         <v>10</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="H66" s="5">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I66" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Location with require shipment</v>
+        <v>[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
       <c r="J66" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Location with require shipment</v>
+        <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C67" s="10"/>
       <c r="D67" s="10" t="s">
@@ -2286,23 +2351,23 @@
         <v>10</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H67" s="5">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I67" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user with no allowance</v>
+        <v>[GIVEN] Location with require shipment</v>
       </c>
       <c r="J67" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
+        <v>//[GIVEN] Location with require shipment</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C68" s="10"/>
       <c r="D68" s="10" t="s">
@@ -2312,176 +2377,228 @@
         <v>10</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H68" s="5">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I68" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
       <c r="J68" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C69" s="10"/>
       <c r="D69" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F69" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="H69" s="5">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I69" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Delete warehouse shipment line and select no in confirm</v>
+        <v>[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
       <c r="J69" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Delete warehouse shipment line and select no in confirm</v>
+        <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C70" s="10"/>
       <c r="D70" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F70" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="H70" s="5">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I70" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Error disallowing deletion</v>
+        <v>[WHEN] Delete warehouse shipment line</v>
       </c>
       <c r="J70" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Error disallowing deletion</v>
+        <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D71" s="10"/>
-      <c r="E71" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F71" t="s">
+        <v>12</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="H71" s="5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I71" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0010] Allowed to Delete Shpt. Line is visible</v>
+        <v>[THEN] Error disallowing deletion</v>
       </c>
       <c r="J71" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0010] Allowed to Delete Shpt. Line is visible</v>
+        <v>//[THEN] Error disallowing deletion</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D72" s="10"/>
-      <c r="F72" t="s">
-        <v>10</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>15</v>
+      <c r="E72" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="H72" s="5">
         <v>10</v>
       </c>
       <c r="I72" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user</v>
+        <v>[SCENARIO #0010] "Allowed to Delete Shpt. Line" is not editable on warehouse employees page</v>
       </c>
       <c r="J72" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse employee for current user</v>
+        <v>//[SCENARIO #0010] "Allowed to Delete Shpt. Line" is not editable on warehouse employees page</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C73" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D73" s="10"/>
       <c r="F73" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="H73" s="5">
         <v>10</v>
       </c>
       <c r="I73" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+        <v>[GIVEN] Location</v>
       </c>
       <c r="J73" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+        <v>//[GIVEN] Location</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C74" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D74" s="10"/>
       <c r="F74" t="s">
+        <v>10</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H74" s="5">
+        <v>10</v>
+      </c>
+      <c r="I74" s="6" t="str">
+        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Warehouse employee for current user</v>
+      </c>
+      <c r="J74" s="7" t="str">
+        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Warehouse employee for current user</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D75" s="10"/>
+      <c r="F75" t="s">
+        <v>11</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H75" s="5">
+        <v>10</v>
+      </c>
+      <c r="I75" s="6" t="str">
+        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+      </c>
+      <c r="J75" s="7" t="str">
+        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D76" s="10"/>
+      <c r="F76" t="s">
         <v>12</v>
       </c>
-      <c r="G74" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H74" s="5">
-        <v>10</v>
-      </c>
-      <c r="I74" s="6" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Allowed to Delete Shpt. Line is visible on warehouse employee card</v>
-      </c>
-      <c r="J74" s="7" t="str">
-        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Allowed to Delete Shpt. Line is visible on warehouse employee card</v>
+      <c r="G76" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H76" s="5">
+        <v>10</v>
+      </c>
+      <c r="I76" s="6" t="str">
+        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Allowed to Delete Shpt. Line is not editable on warehouse employees page</v>
+      </c>
+      <c r="J76" s="7" t="str">
+        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Allowed to Delete Shpt. Line is not editable on warehouse employees page</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2493,32 +2610,48 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+  <conditionalFormatting sqref="D1:D30 D38:D1048576">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
-      <formula>"Given"</formula>
+  <conditionalFormatting sqref="F1:F30 F38:F1048576">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+      <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
-      <formula>"Then"</formula>
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="disabled">
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="disabled">
       <formula>NOT(ISERROR(SEARCH("disabled",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="enabled">
+    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="enabled">
       <formula>NOT(ISERROR(SEARCH("enabled",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F31:F37">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Then"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"Given"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31:D37">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Redesign of feature behavior. #1
</commit_message>
<xml_diff>
--- a/VSCode/Blocking Deletion of Warehouse Shipment Lines/Test/atdd.scenarios/ATDD Scenarios - Blocking Deletion of Warehouse Shipment Lines.xlsx
+++ b/VSCode/Blocking Deletion of Warehouse Shipment Lines/Test/atdd.scenarios/ATDD Scenarios - Blocking Deletion of Warehouse Shipment Lines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc van Vugt\OneDrive\Training\Test Automation\Online Crash Course - March 2020\Business Case - Blocking Deletion of Warehouse Shipment Lines\Code\VSCode\Test\atdd.scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{F8751918-6E3E-4045-90EF-D2382E390DBC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{8F113CA0-FAF8-4005-954D-A91E43D44866}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{F8751918-6E3E-4045-90EF-D2382E390DBC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{8EC3391C-0CB9-4DE2-85D6-7F76CCA2BD0A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28050" windowHeight="16440" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
+    <workbookView xWindow="4800" yWindow="4800" windowWidth="15210" windowHeight="11835" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="41">
   <si>
     <t>Feature</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Error disallowing deletion</t>
   </si>
   <si>
-    <t>Delete warehouse shipment line and select yes in confirm</t>
-  </si>
-  <si>
     <t>Delete warehouse shipment line and select no in confirm</t>
   </si>
   <si>
@@ -135,21 +132,12 @@
     <t>Delete  by user with no allowance manually created whse. shpt. line</t>
   </si>
   <si>
-    <t>Delete  by user with allowance automatically created whse. shpt. line with confirmation</t>
-  </si>
-  <si>
-    <t>Allowed to Delete Shpt. Line is editable on warehouse employees page</t>
-  </si>
-  <si>
     <t>Allowed to Delete Shpt. Line is not editable on warehouse employees page</t>
   </si>
   <si>
     <t>"Allowed to Delete Shpt. Line" is not editable on warehouse employees page</t>
   </si>
   <si>
-    <t>"Allowed to Delete Shpt. Line" is editable on warehouse employees page</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -160,6 +148,12 @@
   </si>
   <si>
     <t>Delete  by user with allowance automatically created whse. shpt. Line</t>
+  </si>
+  <si>
+    <t>Delete  by user with allowance automatically created whse. shpt. Line with confirmation</t>
+  </si>
+  <si>
+    <t>Delete warehouse shipment line and selct yes in confirmation</t>
   </si>
 </sst>
 </file>
@@ -716,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B1ED69-5F96-4A81-993F-0E906F475813}">
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,7 +766,7 @@
     </row>
     <row r="2" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -788,12 +782,12 @@
     </row>
     <row r="3" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" s="5">
         <v>1</v>
@@ -809,7 +803,7 @@
     </row>
     <row r="4" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -817,7 +811,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4" s="5">
         <v>1</v>
@@ -833,7 +827,7 @@
     </row>
     <row r="5" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -857,7 +851,7 @@
     </row>
     <row r="6" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -881,7 +875,7 @@
     </row>
     <row r="7" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -905,7 +899,7 @@
     </row>
     <row r="8" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -929,7 +923,7 @@
     </row>
     <row r="9" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -953,14 +947,12 @@
     </row>
     <row r="10" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="10"/>
-      <c r="D10" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D10" s="10"/>
       <c r="E10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H10" s="5">
         <v>2</v>
@@ -976,17 +968,15 @@
     </row>
     <row r="11" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="10"/>
-      <c r="D11" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D11" s="10"/>
       <c r="F11" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H11" s="5">
         <v>2</v>
@@ -1002,12 +992,10 @@
     </row>
     <row r="12" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="10"/>
-      <c r="D12" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D12" s="10"/>
       <c r="F12" t="s">
         <v>10</v>
       </c>
@@ -1028,12 +1016,10 @@
     </row>
     <row r="13" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="10"/>
-      <c r="D13" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D13" s="10"/>
       <c r="F13" t="s">
         <v>10</v>
       </c>
@@ -1054,12 +1040,10 @@
     </row>
     <row r="14" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="10"/>
-      <c r="D14" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D14" s="10"/>
       <c r="F14" t="s">
         <v>10</v>
       </c>
@@ -1080,12 +1064,10 @@
     </row>
     <row r="15" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="10"/>
-      <c r="D15" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D15" s="10"/>
       <c r="F15" t="s">
         <v>11</v>
       </c>
@@ -1106,38 +1088,36 @@
     </row>
     <row r="16" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="10"/>
-      <c r="D16" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D16" s="10"/>
       <c r="F16" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H16" s="5">
         <v>2</v>
       </c>
       <c r="I16" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Error disallowing deletion</v>
+        <v>[THEN] Warehouse shipment line is deleted</v>
       </c>
       <c r="J16" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Error disallowing deletion</v>
+        <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H17" s="5">
         <v>3</v>
@@ -1153,7 +1133,7 @@
     </row>
     <row r="18" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -1161,7 +1141,7 @@
         <v>10</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H18" s="5">
         <v>3</v>
@@ -1177,7 +1157,7 @@
     </row>
     <row r="19" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -1201,7 +1181,7 @@
     </row>
     <row r="20" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -1225,7 +1205,7 @@
     </row>
     <row r="21" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -1249,7 +1229,7 @@
     </row>
     <row r="22" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -1273,7 +1253,7 @@
     </row>
     <row r="23" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -1297,28 +1277,28 @@
     </row>
     <row r="24" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H24" s="5">
         <v>4</v>
       </c>
       <c r="I24" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0004] Delete  by user with allowance automatically created whse. shpt. line with confirmation</v>
+        <v>[SCENARIO #0004] Delete  by user with allowance automatically created whse. shpt. Line</v>
       </c>
       <c r="J24" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0004] Delete  by user with allowance automatically created whse. shpt. line with confirmation</v>
+        <v>//[SCENARIO #0004] Delete  by user with allowance automatically created whse. shpt. Line</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -1326,7 +1306,7 @@
         <v>10</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H25" s="5">
         <v>4</v>
@@ -1342,7 +1322,7 @@
     </row>
     <row r="26" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -1366,7 +1346,7 @@
     </row>
     <row r="27" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -1390,7 +1370,7 @@
     </row>
     <row r="28" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -1414,7 +1394,7 @@
     </row>
     <row r="29" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -1422,23 +1402,23 @@
         <v>11</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="H29" s="5">
         <v>4</v>
       </c>
       <c r="I29" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Delete warehouse shipment line and select yes in confirm</v>
+        <v>[WHEN] Delete warehouse shipment line</v>
       </c>
       <c r="J29" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Delete warehouse shipment line and select yes in confirm</v>
+        <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -1462,360 +1442,350 @@
     </row>
     <row r="31" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="10"/>
       <c r="E31" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H31" s="5">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I31" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0011] Delete by user with allowance automatically created whse. shpt. line with no confirmation</v>
+        <v>[SCENARIO #0009] "Allowed to Delete Shpt. Line" is not editable on warehouse employees page</v>
       </c>
       <c r="J31" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0011] Delete by user with allowance automatically created whse. shpt. line with no confirmation</v>
+        <v>//[SCENARIO #0009] "Allowed to Delete Shpt. Line" is not editable on warehouse employees page</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="10"/>
       <c r="F32" t="s">
         <v>10</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H32" s="5">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I32" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+        <v>[GIVEN] Location</v>
       </c>
       <c r="J32" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+        <v>//[GIVEN] Location</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="10"/>
       <c r="F33" t="s">
         <v>10</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H33" s="5">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I33" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Location with require shipment</v>
+        <v>[GIVEN] Warehouse employee for current user</v>
       </c>
       <c r="J33" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Location with require shipment</v>
+        <v>//[GIVEN] Warehouse employee for current user</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="10"/>
       <c r="F34" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H34" s="5">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I34" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user with no allowance</v>
+        <v>[WHEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
       <c r="J34" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
+        <v>//[WHEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="10"/>
       <c r="F35" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="H35" s="5">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I35" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>[THEN] Allowed to Delete Shpt. Line is not editable on warehouse employees page</v>
       </c>
       <c r="J35" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>//[THEN] Allowed to Delete Shpt. Line is not editable on warehouse employees page</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="10"/>
-      <c r="D36" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H36" s="5">
-        <v>11</v>
-      </c>
+      <c r="D36" s="10"/>
       <c r="I36" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Delete warehouse shipment line and select no in confirm</v>
+        <v>[FEATURE] Unblock Deletion of Whse. Shpt. Line disabled/</v>
       </c>
       <c r="J36" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Delete warehouse shipment line and select no in confirm</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>//[FEATURE] Unblock Deletion of Whse. Shpt. Line disabled/</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C37" s="10"/>
-      <c r="D37" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>41</v>
+      <c r="D37" s="10"/>
+      <c r="E37" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="H37" s="5">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="I37" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Empty error occurred</v>
+        <v>[SCENARIO #0005] Delete  by user with no allowance manually created whse. shpt. line</v>
       </c>
       <c r="J37" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Empty error occurred</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>//[SCENARIO #0005] Delete  by user with no allowance manually created whse. shpt. line</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="C38" s="10"/>
       <c r="D38" s="10"/>
-      <c r="E38" s="3" t="s">
-        <v>38</v>
+      <c r="F38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="H38" s="5">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I38" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0009] "Allowed to Delete Shpt. Line" is editable on warehouse employees page</v>
+        <v>[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
       <c r="J38" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0009] "Allowed to Delete Shpt. Line" is editable on warehouse employees page</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="C39" s="10"/>
       <c r="D39" s="10"/>
       <c r="F39" t="s">
         <v>10</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="H39" s="5">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I39" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Location</v>
+        <v>[GIVEN] Location with require shipment</v>
       </c>
       <c r="J39" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Location</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>//[GIVEN] Location with require shipment</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="C40" s="10"/>
       <c r="D40" s="10"/>
       <c r="F40" t="s">
         <v>10</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H40" s="5">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I40" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user</v>
+        <v>[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
       <c r="J40" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse employee for current user</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>//[GIVEN] Warehouse employee for current user with allowance</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="C41" s="10"/>
       <c r="D41" s="10"/>
       <c r="F41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="H41" s="5">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I41" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+        <v>[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
       <c r="J41" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>//[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="C42" s="10"/>
       <c r="D42" s="10"/>
       <c r="F42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H42" s="5">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I42" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Allowed to Delete Shpt. Line is editable on warehouse employees page</v>
+        <v>[WHEN] Delete warehouse shipment line</v>
       </c>
       <c r="J42" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Allowed to Delete Shpt. Line is editable on warehouse employees page</v>
+        <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
+      <c r="F43" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H43" s="5">
+        <v>5</v>
+      </c>
       <c r="I43" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[FEATURE] Unblock Deletion of Whse. Shpt. Line disabled/</v>
+        <v>[THEN] Warehouse shipment line is deleted</v>
       </c>
       <c r="J43" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[FEATURE] Unblock Deletion of Whse. Shpt. Line disabled/</v>
+        <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
+      <c r="D44" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="E44" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H44" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I44" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0005] Delete  by user with no allowance manually created whse. shpt. line</v>
+        <v>[SCENARIO #0006] Delete by user with no allowance automatically created whse. shpt. line</v>
       </c>
       <c r="J44" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0005] Delete  by user with no allowance manually created whse. shpt. line</v>
+        <v>//[SCENARIO #0006] Delete by user with no allowance automatically created whse. shpt. line</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
+      <c r="D45" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F45" t="s">
         <v>10</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H45" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I45" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
@@ -1828,10 +1798,12 @@
     </row>
     <row r="46" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
+      <c r="D46" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F46" t="s">
         <v>10</v>
       </c>
@@ -1839,7 +1811,7 @@
         <v>14</v>
       </c>
       <c r="H46" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I46" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
@@ -1852,58 +1824,64 @@
     </row>
     <row r="47" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
+      <c r="D47" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F47" t="s">
         <v>10</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H47" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I47" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user with allowance</v>
+        <v>[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
       <c r="J47" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse employee for current user with allowance</v>
+        <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
+      <c r="D48" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F48" t="s">
         <v>10</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H48" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I48" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
       <c r="J48" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
+      <c r="D49" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F49" t="s">
         <v>11</v>
       </c>
@@ -1911,7 +1889,7 @@
         <v>17</v>
       </c>
       <c r="H49" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I49" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
@@ -1924,67 +1902,65 @@
     </row>
     <row r="50" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
+      <c r="D50" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F50" t="s">
         <v>12</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H50" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I50" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Warehouse shipment line is deleted</v>
+        <v>[THEN] Error disallowing deletion</v>
       </c>
       <c r="J50" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Warehouse shipment line is deleted</v>
+        <v>//[THEN] Error disallowing deletion</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C51" s="10"/>
-      <c r="D51" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D51" s="10"/>
       <c r="E51" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H51" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I51" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0006] Delete by user with no allowance automatically created whse. shpt. line</v>
+        <v>[SCENARIO #0007] Delete by user with allowance manually created whse. shpt. line</v>
       </c>
       <c r="J51" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0006] Delete by user with no allowance automatically created whse. shpt. line</v>
+        <v>//[SCENARIO #0007] Delete by user with allowance manually created whse. shpt. line</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C52" s="10"/>
-      <c r="D52" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D52" s="10"/>
       <c r="F52" t="s">
         <v>10</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H52" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I52" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
@@ -1997,12 +1973,10 @@
     </row>
     <row r="53" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C53" s="10"/>
-      <c r="D53" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D53" s="10"/>
       <c r="F53" t="s">
         <v>10</v>
       </c>
@@ -2010,7 +1984,7 @@
         <v>14</v>
       </c>
       <c r="H53" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I53" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
@@ -2023,64 +1997,58 @@
     </row>
     <row r="54" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C54" s="10"/>
-      <c r="D54" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D54" s="10"/>
       <c r="F54" t="s">
         <v>10</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H54" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I54" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user with no allowance</v>
+        <v>[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
       <c r="J54" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
+        <v>//[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C55" s="10"/>
-      <c r="D55" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D55" s="10"/>
       <c r="F55" t="s">
         <v>10</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H55" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I55" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
       <c r="J55" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>//[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C56" s="10"/>
-      <c r="D56" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D56" s="10"/>
       <c r="F56" t="s">
         <v>11</v>
       </c>
@@ -2088,7 +2056,7 @@
         <v>17</v>
       </c>
       <c r="H56" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I56" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
@@ -2101,65 +2069,67 @@
     </row>
     <row r="57" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C57" s="10"/>
-      <c r="D57" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="D57" s="10"/>
       <c r="F57" t="s">
         <v>12</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H57" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I57" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Error disallowing deletion</v>
+        <v>[THEN] Warehouse shipment line is deleted</v>
       </c>
       <c r="J57" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Error disallowing deletion</v>
+        <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
+      <c r="D58" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="E58" s="3" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H58" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I58" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0007] Delete by user with allowance manually created whse. shpt. line</v>
+        <v>[SCENARIO #0008] Delete  by user with allowance automatically created whse. shpt. Line with confirmation</v>
       </c>
       <c r="J58" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0007] Delete by user with allowance manually created whse. shpt. line</v>
+        <v>//[SCENARIO #0008] Delete  by user with allowance automatically created whse. shpt. Line with confirmation</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
+      <c r="D59" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F59" t="s">
         <v>10</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H59" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I59" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
@@ -2172,10 +2142,12 @@
     </row>
     <row r="60" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
+      <c r="D60" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F60" t="s">
         <v>10</v>
       </c>
@@ -2183,7 +2155,7 @@
         <v>14</v>
       </c>
       <c r="H60" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I60" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
@@ -2196,82 +2168,90 @@
     </row>
     <row r="61" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
+      <c r="D61" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F61" t="s">
         <v>10</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H61" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I61" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user with allowance</v>
+        <v>[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
       <c r="J61" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse employee for current user with allowance</v>
+        <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
+      <c r="D62" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F62" t="s">
         <v>10</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H62" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I62" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
       <c r="J62" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
+      <c r="D63" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F63" t="s">
         <v>11</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="H63" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I63" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Delete warehouse shipment line</v>
+        <v>[WHEN] Delete warehouse shipment line and selct yes in confirmation</v>
       </c>
       <c r="J63" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Delete warehouse shipment line</v>
+        <v>//[WHEN] Delete warehouse shipment line and selct yes in confirmation</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
+      <c r="D64" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="F64" t="s">
         <v>12</v>
       </c>
@@ -2279,7 +2259,7 @@
         <v>18</v>
       </c>
       <c r="H64" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I64" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
@@ -2290,32 +2270,32 @@
         <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C65" s="10"/>
       <c r="D65" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H65" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I65" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0008] Delete  by user with allowance automatically created whse. shpt. Line</v>
+        <v>[SCENARIO #0011] Delete by user with allowance automatically created whse. shpt. line with no confirmation</v>
       </c>
       <c r="J65" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0008] Delete  by user with allowance automatically created whse. shpt. Line</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>//[SCENARIO #0011] Delete by user with allowance automatically created whse. shpt. line with no confirmation</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C66" s="10"/>
       <c r="D66" s="10" t="s">
@@ -2325,23 +2305,23 @@
         <v>10</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H66" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I66" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+        <v>[GIVEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
       <c r="J66" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>//[GIVEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C67" s="10"/>
       <c r="D67" s="10" t="s">
@@ -2354,7 +2334,7 @@
         <v>14</v>
       </c>
       <c r="H67" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I67" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
@@ -2365,9 +2345,9 @@
         <v>//[GIVEN] Location with require shipment</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C68" s="10"/>
       <c r="D68" s="10" t="s">
@@ -2380,7 +2360,7 @@
         <v>20</v>
       </c>
       <c r="H68" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I68" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
@@ -2391,9 +2371,9 @@
         <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C69" s="10"/>
       <c r="D69" s="10" t="s">
@@ -2406,7 +2386,7 @@
         <v>19</v>
       </c>
       <c r="H69" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I69" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
@@ -2417,9 +2397,9 @@
         <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C70" s="10"/>
       <c r="D70" s="10" t="s">
@@ -2429,23 +2409,23 @@
         <v>11</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H70" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I70" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Delete warehouse shipment line</v>
+        <v>[WHEN] Delete warehouse shipment line and select no in confirm</v>
       </c>
       <c r="J70" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Delete warehouse shipment line</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>//[WHEN] Delete warehouse shipment line and select no in confirm</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C71" s="10"/>
       <c r="D71" s="10" t="s">
@@ -2455,30 +2435,30 @@
         <v>12</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="H71" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I71" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Error disallowing deletion</v>
+        <v>[THEN] Empty error occurred</v>
       </c>
       <c r="J71" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Error disallowing deletion</v>
+        <v>//[THEN] Empty error occurred</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D72" s="10"/>
       <c r="E72" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H72" s="5">
         <v>10</v>
@@ -2494,7 +2474,7 @@
     </row>
     <row r="73" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C73" s="10" t="s">
         <v>13</v>
@@ -2504,7 +2484,7 @@
         <v>10</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H73" s="5">
         <v>10</v>
@@ -2520,7 +2500,7 @@
     </row>
     <row r="74" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C74" s="10" t="s">
         <v>13</v>
@@ -2546,7 +2526,7 @@
     </row>
     <row r="75" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C75" s="10" t="s">
         <v>13</v>
@@ -2556,7 +2536,7 @@
         <v>11</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H75" s="5">
         <v>10</v>
@@ -2572,7 +2552,7 @@
     </row>
     <row r="76" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C76" s="10" t="s">
         <v>13</v>
@@ -2582,7 +2562,7 @@
         <v>12</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H76" s="5">
         <v>10</v>
@@ -2614,12 +2594,12 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D30 D38:D1048576">
+  <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F30 F38:F1048576">
+  <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
@@ -2638,7 +2618,7 @@
       <formula>NOT(ISERROR(SEARCH("enabled",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F31:F37">
+  <conditionalFormatting sqref="F65:F71">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
@@ -2649,7 +2629,7 @@
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31:D37">
+  <conditionalFormatting sqref="D65:D71">
     <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Corrected typo Manualy to Manually. #1
</commit_message>
<xml_diff>
--- a/VSCode/Blocking Deletion of Warehouse Shipment Lines/Test/atdd.scenarios/ATDD Scenarios - Blocking Deletion of Warehouse Shipment Lines.xlsx
+++ b/VSCode/Blocking Deletion of Warehouse Shipment Lines/Test/atdd.scenarios/ATDD Scenarios - Blocking Deletion of Warehouse Shipment Lines.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc van Vugt\OneDrive\Training\Test Automation\Online Crash Course - March 2020\Business Case - Blocking Deletion of Warehouse Shipment Lines\Code\VSCode\Test\atdd.scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc van Vugt\OneDrive\Training\Test Automation\Online Crash Course - March 2020\1. March 2020\Sessions 2-6\Session 2\Business Case - Blocking Deletion of Warehouse Shipment Lines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{F8751918-6E3E-4045-90EF-D2382E390DBC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{8EC3391C-0CB9-4DE2-85D6-7F76CCA2BD0A}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{F8751918-6E3E-4045-90EF-D2382E390DBC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{F27F91B7-2500-452B-85C4-2B60A6FD2656}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="4800" windowWidth="15210" windowHeight="11835" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
+    <workbookView xWindow="3375" yWindow="3375" windowWidth="20910" windowHeight="11835" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>Warehouse employee for current user</t>
   </si>
   <si>
-    <t>Manualy created warehouse shipment from released sales order with one line with require shipment location</t>
-  </si>
-  <si>
     <t>Delete warehouse shipment line</t>
   </si>
   <si>
@@ -153,7 +150,10 @@
     <t>Delete  by user with allowance automatically created whse. shpt. Line with confirmation</t>
   </si>
   <si>
-    <t>Delete warehouse shipment line and selct yes in confirmation</t>
+    <t>Delete warehouse shipment line and select yes in confirmation</t>
+  </si>
+  <si>
+    <t>Manually created warehouse shipment from released sales order with one line with require shipment location</t>
   </si>
 </sst>
 </file>
@@ -234,6 +234,54 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -326,54 +374,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -388,24 +388,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:K76" totalsRowShown="0" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:K76" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A1:K76" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{8363E7FF-10AC-4A2B-AF58-2B6F4A3A2982}" name="Feature" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{47ED26B9-CBC1-4AA1-A3A9-843BF13AA89B}" name="Sub Feature" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{FC90C2DF-011C-4E76-8C03-6E75B2478287}" name="Positive-negative" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{8363E7FF-10AC-4A2B-AF58-2B6F4A3A2982}" name="Feature" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{47ED26B9-CBC1-4AA1-A3A9-843BF13AA89B}" name="Sub Feature" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{FC90C2DF-011C-4E76-8C03-6E75B2478287}" name="Positive-negative" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{824F4994-529B-42E7-960A-C52362C8177D}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="13">
+    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="2">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="12">
+    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B1ED69-5F96-4A81-993F-0E906F475813}">
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +740,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -766,7 +766,7 @@
     </row>
     <row r="2" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -782,12 +782,12 @@
     </row>
     <row r="3" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H3" s="5">
         <v>1</v>
@@ -803,7 +803,7 @@
     </row>
     <row r="4" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -811,7 +811,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="5">
         <v>1</v>
@@ -827,7 +827,7 @@
     </row>
     <row r="5" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -851,7 +851,7 @@
     </row>
     <row r="6" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -859,7 +859,7 @@
         <v>10</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" s="5">
         <v>1</v>
@@ -875,7 +875,7 @@
     </row>
     <row r="7" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -883,23 +883,23 @@
         <v>10</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="H7" s="5">
         <v>1</v>
       </c>
       <c r="I7" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>[GIVEN] Manually created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
       <c r="J7" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>//[GIVEN] Manually created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -907,7 +907,7 @@
         <v>11</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" s="5">
         <v>1</v>
@@ -923,7 +923,7 @@
     </row>
     <row r="9" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -931,7 +931,7 @@
         <v>12</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H9" s="5">
         <v>1</v>
@@ -947,12 +947,12 @@
     </row>
     <row r="10" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H10" s="5">
         <v>2</v>
@@ -968,7 +968,7 @@
     </row>
     <row r="11" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -976,7 +976,7 @@
         <v>10</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11" s="5">
         <v>2</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="12" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="13" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -1024,7 +1024,7 @@
         <v>10</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H13" s="5">
         <v>2</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="14" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -1048,7 +1048,7 @@
         <v>10</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H14" s="5">
         <v>2</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="15" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -1072,7 +1072,7 @@
         <v>11</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H15" s="5">
         <v>2</v>
@@ -1088,7 +1088,7 @@
     </row>
     <row r="16" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -1096,7 +1096,7 @@
         <v>12</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H16" s="5">
         <v>2</v>
@@ -1112,12 +1112,12 @@
     </row>
     <row r="17" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H17" s="5">
         <v>3</v>
@@ -1133,7 +1133,7 @@
     </row>
     <row r="18" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -1141,7 +1141,7 @@
         <v>10</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H18" s="5">
         <v>3</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="19" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="20" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -1189,7 +1189,7 @@
         <v>10</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H20" s="5">
         <v>3</v>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="21" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -1213,23 +1213,23 @@
         <v>10</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="H21" s="5">
         <v>3</v>
       </c>
       <c r="I21" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>[GIVEN] Manually created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
       <c r="J21" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>//[GIVEN] Manually created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -1237,7 +1237,7 @@
         <v>11</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H22" s="5">
         <v>3</v>
@@ -1253,7 +1253,7 @@
     </row>
     <row r="23" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -1261,7 +1261,7 @@
         <v>12</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H23" s="5">
         <v>3</v>
@@ -1277,12 +1277,12 @@
     </row>
     <row r="24" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H24" s="5">
         <v>4</v>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="25" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -1306,7 +1306,7 @@
         <v>10</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H25" s="5">
         <v>4</v>
@@ -1322,7 +1322,7 @@
     </row>
     <row r="26" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -1346,7 +1346,7 @@
     </row>
     <row r="27" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -1354,7 +1354,7 @@
         <v>10</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H27" s="5">
         <v>4</v>
@@ -1370,7 +1370,7 @@
     </row>
     <row r="28" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -1378,7 +1378,7 @@
         <v>10</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H28" s="5">
         <v>4</v>
@@ -1394,7 +1394,7 @@
     </row>
     <row r="29" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -1402,7 +1402,7 @@
         <v>11</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H29" s="5">
         <v>4</v>
@@ -1418,7 +1418,7 @@
     </row>
     <row r="30" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -1426,7 +1426,7 @@
         <v>12</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H30" s="5">
         <v>4</v>
@@ -1442,14 +1442,14 @@
     </row>
     <row r="31" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H31" s="5">
         <v>9</v>
@@ -1465,7 +1465,7 @@
     </row>
     <row r="32" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>13</v>
@@ -1475,7 +1475,7 @@
         <v>10</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H32" s="5">
         <v>9</v>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="33" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>13</v>
@@ -1517,7 +1517,7 @@
     </row>
     <row r="34" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>13</v>
@@ -1527,7 +1527,7 @@
         <v>11</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H34" s="5">
         <v>9</v>
@@ -1543,7 +1543,7 @@
     </row>
     <row r="35" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>13</v>
@@ -1553,7 +1553,7 @@
         <v>12</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H35" s="5">
         <v>9</v>
@@ -1569,7 +1569,7 @@
     </row>
     <row r="36" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -1584,12 +1584,12 @@
     </row>
     <row r="37" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H37" s="5">
         <v>5</v>
@@ -1605,7 +1605,7 @@
     </row>
     <row r="38" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
@@ -1613,7 +1613,7 @@
         <v>10</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H38" s="5">
         <v>5</v>
@@ -1629,7 +1629,7 @@
     </row>
     <row r="39" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -1653,7 +1653,7 @@
     </row>
     <row r="40" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
@@ -1661,7 +1661,7 @@
         <v>10</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H40" s="5">
         <v>5</v>
@@ -1677,7 +1677,7 @@
     </row>
     <row r="41" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
@@ -1685,23 +1685,23 @@
         <v>10</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="H41" s="5">
         <v>5</v>
       </c>
       <c r="I41" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>[GIVEN] Manually created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
       <c r="J41" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>//[GIVEN] Manually created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
@@ -1709,7 +1709,7 @@
         <v>11</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H42" s="5">
         <v>5</v>
@@ -1725,7 +1725,7 @@
     </row>
     <row r="43" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
@@ -1733,7 +1733,7 @@
         <v>12</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H43" s="5">
         <v>5</v>
@@ -1749,14 +1749,14 @@
     </row>
     <row r="44" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H44" s="5">
         <v>6</v>
@@ -1772,7 +1772,7 @@
     </row>
     <row r="45" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="10" t="s">
@@ -1782,7 +1782,7 @@
         <v>10</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H45" s="5">
         <v>6</v>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="46" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="10" t="s">
@@ -1824,7 +1824,7 @@
     </row>
     <row r="47" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="10" t="s">
@@ -1834,7 +1834,7 @@
         <v>10</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H47" s="5">
         <v>6</v>
@@ -1850,7 +1850,7 @@
     </row>
     <row r="48" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="10" t="s">
@@ -1860,7 +1860,7 @@
         <v>10</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H48" s="5">
         <v>6</v>
@@ -1876,7 +1876,7 @@
     </row>
     <row r="49" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10" t="s">
@@ -1886,7 +1886,7 @@
         <v>11</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H49" s="5">
         <v>6</v>
@@ -1902,7 +1902,7 @@
     </row>
     <row r="50" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10" t="s">
@@ -1912,7 +1912,7 @@
         <v>12</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H50" s="5">
         <v>6</v>
@@ -1928,12 +1928,12 @@
     </row>
     <row r="51" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
       <c r="E51" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H51" s="5">
         <v>7</v>
@@ -1949,7 +1949,7 @@
     </row>
     <row r="52" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
@@ -1957,7 +1957,7 @@
         <v>10</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H52" s="5">
         <v>7</v>
@@ -1973,7 +1973,7 @@
     </row>
     <row r="53" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
@@ -1997,7 +1997,7 @@
     </row>
     <row r="54" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
@@ -2005,7 +2005,7 @@
         <v>10</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H54" s="5">
         <v>7</v>
@@ -2021,7 +2021,7 @@
     </row>
     <row r="55" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
@@ -2029,23 +2029,23 @@
         <v>10</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="H55" s="5">
         <v>7</v>
       </c>
       <c r="I55" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>[GIVEN] Manually created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
       <c r="J55" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Manualy created warehouse shipment from released sales order with one line with require shipment location</v>
+        <v>//[GIVEN] Manually created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
@@ -2053,7 +2053,7 @@
         <v>11</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H56" s="5">
         <v>7</v>
@@ -2069,7 +2069,7 @@
     </row>
     <row r="57" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
@@ -2077,7 +2077,7 @@
         <v>12</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H57" s="5">
         <v>7</v>
@@ -2093,14 +2093,14 @@
     </row>
     <row r="58" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C58" s="10"/>
       <c r="D58" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H58" s="5">
         <v>8</v>
@@ -2116,7 +2116,7 @@
     </row>
     <row r="59" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C59" s="10"/>
       <c r="D59" s="10" t="s">
@@ -2126,7 +2126,7 @@
         <v>10</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H59" s="5">
         <v>8</v>
@@ -2142,7 +2142,7 @@
     </row>
     <row r="60" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C60" s="10"/>
       <c r="D60" s="10" t="s">
@@ -2168,7 +2168,7 @@
     </row>
     <row r="61" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="10" t="s">
@@ -2178,7 +2178,7 @@
         <v>10</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H61" s="5">
         <v>8</v>
@@ -2194,7 +2194,7 @@
     </row>
     <row r="62" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C62" s="10"/>
       <c r="D62" s="10" t="s">
@@ -2204,7 +2204,7 @@
         <v>10</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H62" s="5">
         <v>8</v>
@@ -2220,7 +2220,7 @@
     </row>
     <row r="63" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C63" s="10"/>
       <c r="D63" s="10" t="s">
@@ -2230,23 +2230,23 @@
         <v>11</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H63" s="5">
         <v>8</v>
       </c>
       <c r="I63" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Delete warehouse shipment line and selct yes in confirmation</v>
+        <v>[WHEN] Delete warehouse shipment line and select yes in confirmation</v>
       </c>
       <c r="J63" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Delete warehouse shipment line and selct yes in confirmation</v>
+        <v>//[WHEN] Delete warehouse shipment line and select yes in confirmation</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C64" s="10"/>
       <c r="D64" s="10" t="s">
@@ -2256,7 +2256,7 @@
         <v>12</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H64" s="5">
         <v>8</v>
@@ -2272,14 +2272,14 @@
     </row>
     <row r="65" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C65" s="10"/>
       <c r="D65" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H65" s="5">
         <v>11</v>
@@ -2295,7 +2295,7 @@
     </row>
     <row r="66" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C66" s="10"/>
       <c r="D66" s="10" t="s">
@@ -2305,7 +2305,7 @@
         <v>10</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H66" s="5">
         <v>11</v>
@@ -2321,7 +2321,7 @@
     </row>
     <row r="67" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C67" s="10"/>
       <c r="D67" s="10" t="s">
@@ -2347,7 +2347,7 @@
     </row>
     <row r="68" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C68" s="10"/>
       <c r="D68" s="10" t="s">
@@ -2357,7 +2357,7 @@
         <v>10</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H68" s="5">
         <v>11</v>
@@ -2373,7 +2373,7 @@
     </row>
     <row r="69" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C69" s="10"/>
       <c r="D69" s="10" t="s">
@@ -2383,7 +2383,7 @@
         <v>10</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H69" s="5">
         <v>11</v>
@@ -2399,7 +2399,7 @@
     </row>
     <row r="70" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C70" s="10"/>
       <c r="D70" s="10" t="s">
@@ -2409,7 +2409,7 @@
         <v>11</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H70" s="5">
         <v>11</v>
@@ -2425,7 +2425,7 @@
     </row>
     <row r="71" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C71" s="10"/>
       <c r="D71" s="10" t="s">
@@ -2435,7 +2435,7 @@
         <v>12</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H71" s="5">
         <v>11</v>
@@ -2451,14 +2451,14 @@
     </row>
     <row r="72" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D72" s="10"/>
       <c r="E72" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H72" s="5">
         <v>10</v>
@@ -2474,7 +2474,7 @@
     </row>
     <row r="73" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C73" s="10" t="s">
         <v>13</v>
@@ -2484,7 +2484,7 @@
         <v>10</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H73" s="5">
         <v>10</v>
@@ -2500,7 +2500,7 @@
     </row>
     <row r="74" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C74" s="10" t="s">
         <v>13</v>
@@ -2526,7 +2526,7 @@
     </row>
     <row r="75" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C75" s="10" t="s">
         <v>13</v>
@@ -2536,7 +2536,7 @@
         <v>11</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H75" s="5">
         <v>10</v>
@@ -2552,7 +2552,7 @@
     </row>
     <row r="76" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C76" s="10" t="s">
         <v>13</v>
@@ -2562,7 +2562,7 @@
         <v>12</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H76" s="5">
         <v>10</v>
@@ -2590,47 +2590,47 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="disabled">
+    <cfRule type="containsText" dxfId="16" priority="9" operator="containsText" text="disabled">
       <formula>NOT(ISERROR(SEARCH("disabled",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="enabled">
+    <cfRule type="containsText" dxfId="15" priority="10" operator="containsText" text="enabled">
       <formula>NOT(ISERROR(SEARCH("enabled",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F65:F71">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:D71">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed type in scenarion 5/8/11. #1
</commit_message>
<xml_diff>
--- a/VSCode/Blocking Deletion of Warehouse Shipment Lines/Test/atdd.scenarios/ATDD Scenarios - Blocking Deletion of Warehouse Shipment Lines.xlsx
+++ b/VSCode/Blocking Deletion of Warehouse Shipment Lines/Test/atdd.scenarios/ATDD Scenarios - Blocking Deletion of Warehouse Shipment Lines.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc van Vugt\OneDrive\Training\Test Automation\Online Crash Course - March 2020\1. March 2020\Sessions 2-6\Session 2\Business Case - Blocking Deletion of Warehouse Shipment Lines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc van Vugt\source\repos\Test-Automation-Examples\VSCode\Blocking Deletion of Warehouse Shipment Lines\Test\atdd.scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{F8751918-6E3E-4045-90EF-D2382E390DBC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{F27F91B7-2500-452B-85C4-2B60A6FD2656}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D391D6-22A8-417A-891F-7088943F1F0E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3375" yWindow="3375" windowWidth="20910" windowHeight="11835" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B1ED69-5F96-4A81-993F-0E906F475813}">
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,18 +1661,18 @@
         <v>10</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H40" s="5">
         <v>5</v>
       </c>
       <c r="I40" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user with allowance</v>
+        <v>[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
       <c r="J40" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse employee for current user with allowance</v>
+        <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2178,18 +2178,18 @@
         <v>10</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H61" s="5">
         <v>8</v>
       </c>
       <c r="I61" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user with no allowance</v>
+        <v>[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
       <c r="J61" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
+        <v>//[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2357,18 +2357,18 @@
         <v>10</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H68" s="5">
         <v>11</v>
       </c>
       <c r="I68" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user with no allowance</v>
+        <v>[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
       <c r="J68" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
+        <v>//[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update on ATDD sheet. #1
</commit_message>
<xml_diff>
--- a/VSCode/Blocking Deletion of Warehouse Shipment Lines/Test/atdd.scenarios/ATDD Scenarios - Blocking Deletion of Warehouse Shipment Lines.xlsx
+++ b/VSCode/Blocking Deletion of Warehouse Shipment Lines/Test/atdd.scenarios/ATDD Scenarios - Blocking Deletion of Warehouse Shipment Lines.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc van Vugt\source\repos\Test-Automation-Examples\VSCode\Blocking Deletion of Warehouse Shipment Lines\Test\atdd.scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc van Vugt\OneDrive\Training\Test Automation\Online Crash Course\5. May 2020\Sessions 2-6\Session 4\Test Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D391D6-22A8-417A-891F-7088943F1F0E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{73D391D6-22A8-417A-891F-7088943F1F0E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{9AF1EF8B-9AFC-4AB9-BC7B-D5766E95B217}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="44">
   <si>
     <t>Feature</t>
   </si>
@@ -42,6 +42,9 @@
     <t>UI</t>
   </si>
   <si>
+    <t>Positive-negative</t>
+  </si>
+  <si>
     <t>Scenario</t>
   </si>
   <si>
@@ -63,97 +66,103 @@
     <t>Notes</t>
   </si>
   <si>
+    <t>Unblock Deletion of Whse. Shpt. Line enabled</t>
+  </si>
+  <si>
+    <t>Delete by user with no allowance manually created whse. shpt. line</t>
+  </si>
+  <si>
     <t>Given</t>
   </si>
   <si>
+    <t>Enable "Unblock Deletion of Shpt. Line" on warehouse setup</t>
+  </si>
+  <si>
+    <t>Location with require shipment</t>
+  </si>
+  <si>
+    <t>Warehouse employee for current user with no allowance</t>
+  </si>
+  <si>
+    <t>Manually created warehouse shipment from released sales order with one line with require shipment location</t>
+  </si>
+  <si>
     <t>When</t>
   </si>
   <si>
+    <t>Delete warehouse shipment line</t>
+  </si>
+  <si>
     <t>Then</t>
   </si>
   <si>
+    <t>Warehouse shipment line is deleted</t>
+  </si>
+  <si>
+    <t>Delete by user with no allowance automatically created whse. shpt. line</t>
+  </si>
+  <si>
+    <t>Automatically created warehouse shipment from released sales order with one line with require shipment location</t>
+  </si>
+  <si>
+    <t>Delete by user with allowance manually created whse. shpt. line</t>
+  </si>
+  <si>
+    <t>Warehouse employee for current user with allowance</t>
+  </si>
+  <si>
+    <t>[GIVEN] Warehouse employee for current user with allowance</t>
+  </si>
+  <si>
+    <t>[THEN] Warehouse shipment line is deleted</t>
+  </si>
+  <si>
+    <t>Delete  by user with allowance automatically created whse. shpt. line</t>
+  </si>
+  <si>
     <t>X</t>
   </si>
   <si>
-    <t>Location with require shipment</t>
+    <t>"Allowed to Delete Shpt. Line" is not editable on warehouse employees page</t>
+  </si>
+  <si>
+    <t>Location</t>
   </si>
   <si>
     <t>Warehouse employee for current user</t>
   </si>
   <si>
-    <t>Delete warehouse shipment line</t>
-  </si>
-  <si>
-    <t>Warehouse shipment line is deleted</t>
-  </si>
-  <si>
-    <t>Automatically created warehouse shipment from released sales order with one line with require shipment location</t>
-  </si>
-  <si>
-    <t>Warehouse employee for current user with no allowance</t>
-  </si>
-  <si>
-    <t>Warehouse employee for current user with allowance</t>
-  </si>
-  <si>
-    <t>Positive-negative</t>
+    <t>Allowed to Delete Shpt. Line is not editable on warehouse employees page</t>
+  </si>
+  <si>
+    <t>Unblock Deletion of Whse. Shpt. Line disabled</t>
+  </si>
+  <si>
+    <t>Delete  by user with no allowance manually created whse. shpt. line</t>
+  </si>
+  <si>
+    <t>Disable "Unblock Deletion of Shpt. Line" on warehouse setup</t>
   </si>
   <si>
     <t>Error disallowing deletion</t>
   </si>
   <si>
+    <t>Delete  by user with allowance automatically created whse. shpt. Line with confirmation</t>
+  </si>
+  <si>
+    <t>Delete warehouse shipment line and select yes in confirmation</t>
+  </si>
+  <si>
+    <t>Delete by user with allowance automatically created whse. shpt. line with no confirmation</t>
+  </si>
+  <si>
     <t>Delete warehouse shipment line and select no in confirm</t>
   </si>
   <si>
-    <t>Unblock Deletion of Whse. Shpt. Line enabled</t>
-  </si>
-  <si>
-    <t>Unblock Deletion of Whse. Shpt. Line disabled</t>
-  </si>
-  <si>
-    <t>Enable "Unblock Deletion of Shpt. Line" on warehouse setup</t>
-  </si>
-  <si>
-    <t>Disable "Unblock Deletion of Shpt. Line" on warehouse setup</t>
-  </si>
-  <si>
-    <t>Delete by user with no allowance manually created whse. shpt. line</t>
-  </si>
-  <si>
-    <t>Delete by user with no allowance automatically created whse. shpt. line</t>
-  </si>
-  <si>
-    <t>Delete by user with allowance manually created whse. shpt. line</t>
-  </si>
-  <si>
-    <t>Delete  by user with no allowance manually created whse. shpt. line</t>
-  </si>
-  <si>
-    <t>Allowed to Delete Shpt. Line is not editable on warehouse employees page</t>
-  </si>
-  <si>
-    <t>"Allowed to Delete Shpt. Line" is not editable on warehouse employees page</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Delete by user with allowance automatically created whse. shpt. line with no confirmation</t>
-  </si>
-  <si>
     <t>Empty error occurred</t>
   </si>
   <si>
-    <t>Delete  by user with allowance automatically created whse. shpt. Line</t>
-  </si>
-  <si>
-    <t>Delete  by user with allowance automatically created whse. shpt. Line with confirmation</t>
-  </si>
-  <si>
-    <t>Delete warehouse shipment line and select yes in confirmation</t>
-  </si>
-  <si>
-    <t>Manually created warehouse shipment from released sales order with one line with require shipment location</t>
+    <t>FEATURE</t>
   </si>
 </sst>
 </file>
@@ -163,7 +172,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,16 +187,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -195,11 +217,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -229,59 +267,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -374,6 +368,54 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -388,24 +430,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:K76" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:K76" totalsRowShown="0" headerRowDxfId="21">
   <autoFilter ref="A1:K76" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{8363E7FF-10AC-4A2B-AF58-2B6F4A3A2982}" name="Feature" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{47ED26B9-CBC1-4AA1-A3A9-843BF13AA89B}" name="Sub Feature" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{FC90C2DF-011C-4E76-8C03-6E75B2478287}" name="Positive-negative" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{8363E7FF-10AC-4A2B-AF58-2B6F4A3A2982}" name="Feature" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{47ED26B9-CBC1-4AA1-A3A9-843BF13AA89B}" name="Sub Feature" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{FC90C2DF-011C-4E76-8C03-6E75B2478287}" name="Positive-negative" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="16"/>
     <tableColumn id="3" xr3:uid="{824F4994-529B-42E7-960A-C52362C8177D}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="13">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="1">
+    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="12">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -708,13 +750,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B1ED69-5F96-4A81-993F-0E906F475813}">
-  <dimension ref="A1:K76"/>
+  <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
@@ -729,7 +771,7 @@
     <col min="11" max="11" width="8.5703125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -740,37 +782,40 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="F2" s="4"/>
+      <c r="G2" s="11" t="s">
+        <v>43</v>
+      </c>
       <c r="I2" s="4" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[FEATURE] Unblock Deletion of Whse. Shpt. Line enabled/</v>
@@ -780,14 +825,14 @@
         <v>//[FEATURE] Unblock Deletion of Whse. Shpt. Line enabled/</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="3" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="H3" s="5">
         <v>1</v>
@@ -801,17 +846,17 @@
         <v>//[SCENARIO #0001] Delete by user with no allowance manually created whse. shpt. line</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H4" s="5">
         <v>1</v>
@@ -825,17 +870,17 @@
         <v>//[GIVEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H5" s="5">
         <v>1</v>
@@ -849,17 +894,17 @@
         <v>//[GIVEN] Location with require shipment</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H6" s="5">
         <v>1</v>
@@ -873,17 +918,17 @@
         <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="H7" s="5">
         <v>1</v>
@@ -897,17 +942,17 @@
         <v>//[GIVEN] Manually created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H8" s="5">
         <v>1</v>
@@ -921,17 +966,17 @@
         <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H9" s="5">
         <v>1</v>
@@ -947,12 +992,12 @@
     </row>
     <row r="10" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H10" s="5">
         <v>2</v>
@@ -966,17 +1011,17 @@
         <v>//[SCENARIO #0002] Delete by user with no allowance automatically created whse. shpt. line</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H11" s="5">
         <v>2</v>
@@ -990,17 +1035,17 @@
         <v>//[GIVEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H12" s="5">
         <v>2</v>
@@ -1014,17 +1059,17 @@
         <v>//[GIVEN] Location with require shipment</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H13" s="5">
         <v>2</v>
@@ -1038,17 +1083,17 @@
         <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H14" s="5">
         <v>2</v>
@@ -1062,17 +1107,17 @@
         <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H15" s="5">
         <v>2</v>
@@ -1086,17 +1131,17 @@
         <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="F16" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H16" s="5">
         <v>2</v>
@@ -1110,14 +1155,14 @@
         <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="30.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H17" s="5">
         <v>3</v>
@@ -1131,17 +1176,17 @@
         <v>//[SCENARIO #0003] Delete by user with allowance manually created whse. shpt. line</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H18" s="5">
         <v>3</v>
@@ -1155,17 +1200,17 @@
         <v>//[GIVEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H19" s="5">
         <v>3</v>
@@ -1179,41 +1224,40 @@
         <v>//[GIVEN] Location with require shipment</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H20" s="5">
         <v>3</v>
       </c>
-      <c r="I20" s="6" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse employee for current user with allowance</v>
+      <c r="I20" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="J20" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="31.5" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="H21" s="5">
         <v>3</v>
@@ -1227,17 +1271,17 @@
         <v>//[GIVEN] Manually created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H22" s="5">
         <v>3</v>
@@ -1251,62 +1295,61 @@
         <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H23" s="5">
         <v>3</v>
       </c>
-      <c r="I23" s="6" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Warehouse shipment line is deleted</v>
+      <c r="I23" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="J23" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="30.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="H24" s="5">
         <v>4</v>
       </c>
       <c r="I24" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0004] Delete  by user with allowance automatically created whse. shpt. Line</v>
+        <v>[SCENARIO #0004] Delete  by user with allowance automatically created whse. shpt. line</v>
       </c>
       <c r="J24" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0004] Delete  by user with allowance automatically created whse. shpt. Line</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>//[SCENARIO #0004] Delete  by user with allowance automatically created whse. shpt. line</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="F25" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H25" s="5">
         <v>4</v>
@@ -1320,17 +1363,17 @@
         <v>//[GIVEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="F26" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H26" s="5">
         <v>4</v>
@@ -1344,17 +1387,17 @@
         <v>//[GIVEN] Location with require shipment</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="F27" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H27" s="5">
         <v>4</v>
@@ -1368,17 +1411,17 @@
         <v>//[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="F28" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H28" s="5">
         <v>4</v>
@@ -1392,17 +1435,17 @@
         <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="F29" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H29" s="5">
         <v>4</v>
@@ -1416,17 +1459,17 @@
         <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="F30" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H30" s="5">
         <v>4</v>
@@ -1440,16 +1483,16 @@
         <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="30.75" customHeight="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H31" s="5">
         <v>9</v>
@@ -1463,19 +1506,19 @@
         <v>//[SCENARIO #0009] "Allowed to Delete Shpt. Line" is not editable on warehouse employees page</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D32" s="10"/>
       <c r="F32" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H32" s="5">
         <v>9</v>
@@ -1489,19 +1532,19 @@
         <v>//[GIVEN] Location</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D33" s="10"/>
       <c r="F33" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="H33" s="5">
         <v>9</v>
@@ -1515,19 +1558,19 @@
         <v>//[GIVEN] Warehouse employee for current user</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D34" s="10"/>
       <c r="F34" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H34" s="5">
         <v>9</v>
@@ -1541,19 +1584,19 @@
         <v>//[WHEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D35" s="10"/>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H35" s="5">
         <v>9</v>
@@ -1567,12 +1610,15 @@
         <v>//[THEN] Allowed to Delete Shpt. Line is not editable on warehouse employees page</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="29.25" customHeight="1" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
+      <c r="G36" s="11" t="s">
+        <v>43</v>
+      </c>
       <c r="I36" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[FEATURE] Unblock Deletion of Whse. Shpt. Line disabled/</v>
@@ -1582,14 +1628,14 @@
         <v>//[FEATURE] Unblock Deletion of Whse. Shpt. Line disabled/</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H37" s="5">
         <v>5</v>
@@ -1603,17 +1649,17 @@
         <v>//[SCENARIO #0005] Delete  by user with no allowance manually created whse. shpt. line</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
       <c r="F38" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="H38" s="5">
         <v>5</v>
@@ -1627,17 +1673,17 @@
         <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
       <c r="F39" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H39" s="5">
         <v>5</v>
@@ -1651,17 +1697,17 @@
         <v>//[GIVEN] Location with require shipment</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
       <c r="F40" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H40" s="5">
         <v>5</v>
@@ -1675,17 +1721,17 @@
         <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
       <c r="F41" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="H41" s="5">
         <v>5</v>
@@ -1699,17 +1745,17 @@
         <v>//[GIVEN] Manually created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
       <c r="F42" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H42" s="5">
         <v>5</v>
@@ -1723,17 +1769,17 @@
         <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
       <c r="F43" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H43" s="5">
         <v>5</v>
@@ -1747,16 +1793,16 @@
         <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="29.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H44" s="5">
         <v>6</v>
@@ -1770,19 +1816,19 @@
         <v>//[SCENARIO #0006] Delete by user with no allowance automatically created whse. shpt. line</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F45" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="H45" s="5">
         <v>6</v>
@@ -1796,19 +1842,19 @@
         <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F46" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H46" s="5">
         <v>6</v>
@@ -1822,19 +1868,19 @@
         <v>//[GIVEN] Location with require shipment</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F47" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H47" s="5">
         <v>6</v>
@@ -1848,19 +1894,19 @@
         <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F48" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H48" s="5">
         <v>6</v>
@@ -1874,19 +1920,19 @@
         <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F49" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H49" s="5">
         <v>6</v>
@@ -1900,19 +1946,19 @@
         <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F50" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="H50" s="5">
         <v>6</v>
@@ -1926,14 +1972,14 @@
         <v>//[THEN] Error disallowing deletion</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="29.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
       <c r="E51" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H51" s="5">
         <v>7</v>
@@ -1947,17 +1993,17 @@
         <v>//[SCENARIO #0007] Delete by user with allowance manually created whse. shpt. line</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
       <c r="F52" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="H52" s="5">
         <v>7</v>
@@ -1971,17 +2017,17 @@
         <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
       <c r="F53" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H53" s="5">
         <v>7</v>
@@ -1995,17 +2041,17 @@
         <v>//[GIVEN] Location with require shipment</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
       <c r="F54" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H54" s="5">
         <v>7</v>
@@ -2019,17 +2065,17 @@
         <v>//[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
       <c r="F55" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="H55" s="5">
         <v>7</v>
@@ -2043,17 +2089,17 @@
         <v>//[GIVEN] Manually created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
       <c r="F56" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H56" s="5">
         <v>7</v>
@@ -2067,17 +2113,17 @@
         <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
       <c r="F57" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H57" s="5">
         <v>7</v>
@@ -2091,13 +2137,13 @@
         <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="29.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C58" s="10"/>
       <c r="D58" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>38</v>
@@ -2114,19 +2160,19 @@
         <v>//[SCENARIO #0008] Delete  by user with allowance automatically created whse. shpt. Line with confirmation</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C59" s="10"/>
       <c r="D59" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F59" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="H59" s="5">
         <v>8</v>
@@ -2140,19 +2186,19 @@
         <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C60" s="10"/>
       <c r="D60" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F60" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H60" s="5">
         <v>8</v>
@@ -2166,19 +2212,19 @@
         <v>//[GIVEN] Location with require shipment</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F61" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H61" s="5">
         <v>8</v>
@@ -2192,19 +2238,19 @@
         <v>//[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C62" s="10"/>
       <c r="D62" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F62" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H62" s="5">
         <v>8</v>
@@ -2218,16 +2264,16 @@
         <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C63" s="10"/>
       <c r="D63" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F63" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>39</v>
@@ -2244,19 +2290,19 @@
         <v>//[WHEN] Delete warehouse shipment line and select yes in confirmation</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C64" s="10"/>
       <c r="D64" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F64" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H64" s="5">
         <v>8</v>
@@ -2270,16 +2316,16 @@
         <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="30.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C65" s="10"/>
       <c r="D65" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H65" s="5">
         <v>11</v>
@@ -2293,19 +2339,19 @@
         <v>//[SCENARIO #0011] Delete by user with allowance automatically created whse. shpt. line with no confirmation</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C66" s="10"/>
       <c r="D66" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F66" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H66" s="5">
         <v>11</v>
@@ -2319,19 +2365,19 @@
         <v>//[GIVEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C67" s="10"/>
       <c r="D67" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F67" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H67" s="5">
         <v>11</v>
@@ -2345,19 +2391,19 @@
         <v>//[GIVEN] Location with require shipment</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C68" s="10"/>
       <c r="D68" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F68" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H68" s="5">
         <v>11</v>
@@ -2371,19 +2417,19 @@
         <v>//[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C69" s="10"/>
       <c r="D69" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F69" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H69" s="5">
         <v>11</v>
@@ -2397,19 +2443,19 @@
         <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C70" s="10"/>
       <c r="D70" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F70" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="H70" s="5">
         <v>11</v>
@@ -2423,19 +2469,19 @@
         <v>//[WHEN] Delete warehouse shipment line and select no in confirm</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C71" s="10"/>
       <c r="D71" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F71" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H71" s="5">
         <v>11</v>
@@ -2449,16 +2495,16 @@
         <v>//[THEN] Empty error occurred</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="29.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D72" s="10"/>
       <c r="E72" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H72" s="5">
         <v>10</v>
@@ -2472,19 +2518,19 @@
         <v>//[SCENARIO #0010] "Allowed to Delete Shpt. Line" is not editable on warehouse employees page</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D73" s="10"/>
       <c r="F73" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H73" s="5">
         <v>10</v>
@@ -2498,19 +2544,19 @@
         <v>//[GIVEN] Location</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D74" s="10"/>
       <c r="F74" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="H74" s="5">
         <v>10</v>
@@ -2524,19 +2570,19 @@
         <v>//[GIVEN] Warehouse employee for current user</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D75" s="10"/>
       <c r="F75" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="H75" s="5">
         <v>10</v>
@@ -2550,19 +2596,19 @@
         <v>//[WHEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D76" s="10"/>
       <c r="F76" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H76" s="5">
         <v>10</v>
@@ -2576,6 +2622,7 @@
         <v>//[THEN] Allowed to Delete Shpt. Line is not editable on warehouse employees page</v>
       </c>
     </row>
+    <row r="77" spans="1:10" collapsed="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="H1:H1048576">
     <cfRule type="colorScale" priority="30">
@@ -2590,47 +2637,47 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsText" dxfId="16" priority="9" operator="containsText" text="disabled">
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="disabled">
       <formula>NOT(ISERROR(SEARCH("disabled",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="10" operator="containsText" text="enabled">
+    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="enabled">
       <formula>NOT(ISERROR(SEARCH("enabled",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F65:F71">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:D71">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
ATDD Sheet now has ATDD.TestScriptor Format columns. #1
</commit_message>
<xml_diff>
--- a/VSCode/Blocking Deletion of Warehouse Shipment Lines/Test/atdd.scenarios/ATDD Scenarios - Blocking Deletion of Warehouse Shipment Lines.xlsx
+++ b/VSCode/Blocking Deletion of Warehouse Shipment Lines/Test/atdd.scenarios/ATDD Scenarios - Blocking Deletion of Warehouse Shipment Lines.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc van Vugt\OneDrive\Training\Test Automation\Online Crash Course\5. May 2020\Sessions 2-6\Session 4\Test Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc van Vugt\source\repos\Test-Automation-Examples\VSCode\Blocking Deletion of Warehouse Shipment Lines\Test\atdd.scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{73D391D6-22A8-417A-891F-7088943F1F0E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{9AF1EF8B-9AFC-4AB9-BC7B-D5766E95B217}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C20E0EB-2CA4-4C30-84E8-617F516B14A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
+    <workbookView xWindow="29610" yWindow="180" windowWidth="24510" windowHeight="15990" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="45">
   <si>
     <t>Feature</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>FEATURE</t>
+  </si>
+  <si>
+    <t>ATDD.TestScriptor Format</t>
   </si>
 </sst>
 </file>
@@ -172,7 +175,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +197,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="3">
@@ -237,7 +252,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -270,12 +285,39 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -430,24 +472,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:K76" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="A1:K76" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{8363E7FF-10AC-4A2B-AF58-2B6F4A3A2982}" name="Feature" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{47ED26B9-CBC1-4AA1-A3A9-843BF13AA89B}" name="Sub Feature" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{FC90C2DF-011C-4E76-8C03-6E75B2478287}" name="Positive-negative" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:L76" totalsRowShown="0" headerRowDxfId="22">
+  <autoFilter ref="A1:L76" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{8363E7FF-10AC-4A2B-AF58-2B6F4A3A2982}" name="Feature" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{47ED26B9-CBC1-4AA1-A3A9-843BF13AA89B}" name="Sub Feature" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{FC90C2DF-011C-4E76-8C03-6E75B2478287}" name="Positive-negative" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="17"/>
     <tableColumn id="3" xr3:uid="{824F4994-529B-42E7-960A-C52362C8177D}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="13">
+    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="14">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="12">
+    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="13">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{C88A1207-6598-4461-BC21-DEF845DAC115}" name="ATDD.TestScriptor Format" dataDxfId="0">
+      <calculatedColumnFormula>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -750,10 +795,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B1ED69-5F96-4A81-993F-0E906F475813}">
-  <dimension ref="A1:K77"/>
+  <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="8" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -765,13 +811,13 @@
     <col min="5" max="5" width="13.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="58.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="54.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="56.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="5" customWidth="1"/>
+    <col min="9" max="10" width="49.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="49.42578125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -803,10 +849,13 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="30.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -824,8 +873,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[FEATURE] Unblock Deletion of Whse. Shpt. Line enabled/</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Feature 'Unblock Deletion of Whse. Shpt. Line enabled' {</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -845,8 +898,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0001] Delete by user with no allowance manually created whse. shpt. line</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0001 'Delete by user with no allowance manually created whse. shpt. line' {</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -869,8 +926,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Enable "Unblock Deletion of Shpt. Line" on warehouse setup'</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -893,8 +954,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Location with require shipment</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Location with require shipment'</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -917,8 +982,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user with no allowance'</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -941,8 +1010,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Manually created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Manually created warehouse shipment from released sales order with one line with require shipment location'</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
@@ -965,8 +1038,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Delete warehouse shipment line'</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -989,8 +1066,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Warehouse shipment line is deleted' }</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1010,8 +1091,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0002] Delete by user with no allowance automatically created whse. shpt. line</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0002 'Delete by user with no allowance automatically created whse. shpt. line' {</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
@@ -1034,8 +1119,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Enable "Unblock Deletion of Shpt. Line" on warehouse setup'</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -1058,8 +1147,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Location with require shipment</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Location with require shipment'</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -1082,8 +1175,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user with no allowance'</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -1106,8 +1203,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Automatically created warehouse shipment from released sales order with one line with require shipment location'</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
@@ -1130,8 +1231,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Delete warehouse shipment line'</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>11</v>
       </c>
@@ -1154,8 +1259,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="30.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Warehouse shipment line is deleted' }</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
@@ -1175,8 +1284,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0003] Delete by user with allowance manually created whse. shpt. line</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0003 'Delete by user with allowance manually created whse. shpt. line' {</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>11</v>
       </c>
@@ -1199,8 +1312,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Enable "Unblock Deletion of Shpt. Line" on warehouse setup'</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
@@ -1223,8 +1340,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Location with require shipment</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Location with require shipment'</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>11</v>
       </c>
@@ -1246,8 +1367,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="31.5" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K20" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user with allowance'</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>11</v>
       </c>
@@ -1270,8 +1395,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Manually created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Manually created warehouse shipment from released sales order with one line with require shipment location'</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>11</v>
       </c>
@@ -1294,8 +1423,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Delete warehouse shipment line'</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>11</v>
       </c>
@@ -1317,8 +1450,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="30.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Warehouse shipment line is deleted' }</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>11</v>
       </c>
@@ -1338,8 +1475,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0004] Delete  by user with allowance automatically created whse. shpt. line</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K24" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0004 'Delete  by user with allowance automatically created whse. shpt. line' {</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>11</v>
       </c>
@@ -1362,8 +1503,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Enable "Unblock Deletion of Shpt. Line" on warehouse setup'</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>11</v>
       </c>
@@ -1386,8 +1531,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Location with require shipment</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K26" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Location with require shipment'</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>11</v>
       </c>
@@ -1410,8 +1559,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K27" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user with allowance'</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>11</v>
       </c>
@@ -1434,8 +1587,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Automatically created warehouse shipment from released sales order with one line with require shipment location'</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>11</v>
       </c>
@@ -1458,8 +1615,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K29" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Delete warehouse shipment line'</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>11</v>
       </c>
@@ -1482,8 +1643,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="30.75" customHeight="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K30" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Warehouse shipment line is deleted' }</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>11</v>
       </c>
@@ -1505,8 +1670,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0009] "Allowed to Delete Shpt. Line" is not editable on warehouse employees page</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K31" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0009 '"Allowed to Delete Shpt. Line" is not editable on warehouse employees page' {</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>11</v>
       </c>
@@ -1531,8 +1700,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Location</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K32" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Location'</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>11</v>
       </c>
@@ -1557,8 +1730,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Warehouse employee for current user</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K33" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user'</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>11</v>
       </c>
@@ -1583,8 +1760,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K34" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Enable "Unblock Deletion of Shpt. Line" on warehouse setup'</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>11</v>
       </c>
@@ -1609,8 +1790,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Allowed to Delete Shpt. Line is not editable on warehouse employees page</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="29.25" customHeight="1" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K35" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Allowed to Delete Shpt. Line is not editable on warehouse employees page' } }</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>34</v>
       </c>
@@ -1627,8 +1812,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[FEATURE] Unblock Deletion of Whse. Shpt. Line disabled/</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="K36" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Feature 'Unblock Deletion of Whse. Shpt. Line disabled' {</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>34</v>
       </c>
@@ -1648,8 +1837,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0005] Delete  by user with no allowance manually created whse. shpt. line</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K37" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0005 'Delete  by user with no allowance manually created whse. shpt. line' {</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>34</v>
       </c>
@@ -1672,8 +1865,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K38" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Disable "Unblock Deletion of Shpt. Line" on warehouse setup'</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>34</v>
       </c>
@@ -1696,8 +1893,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Location with require shipment</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K39" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Location with require shipment'</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>34</v>
       </c>
@@ -1720,8 +1921,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K40" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user with no allowance'</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>34</v>
       </c>
@@ -1744,8 +1949,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Manually created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K41" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Manually created warehouse shipment from released sales order with one line with require shipment location'</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>34</v>
       </c>
@@ -1768,8 +1977,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K42" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Delete warehouse shipment line'</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>34</v>
       </c>
@@ -1792,8 +2005,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" ht="29.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="K43" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Warehouse shipment line is deleted' }</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>34</v>
       </c>
@@ -1815,8 +2032,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0006] Delete by user with no allowance automatically created whse. shpt. line</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K44" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0006 'Delete by user with no allowance automatically created whse. shpt. line' {</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>34</v>
       </c>
@@ -1841,8 +2062,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K45" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Disable "Unblock Deletion of Shpt. Line" on warehouse setup'</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>34</v>
       </c>
@@ -1867,8 +2092,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Location with require shipment</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K46" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Location with require shipment'</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>34</v>
       </c>
@@ -1893,8 +2122,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Warehouse employee for current user with no allowance</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K47" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user with no allowance'</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>34</v>
       </c>
@@ -1919,8 +2152,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K48" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Automatically created warehouse shipment from released sales order with one line with require shipment location'</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>34</v>
       </c>
@@ -1945,8 +2182,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K49" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Delete warehouse shipment line'</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>34</v>
       </c>
@@ -1971,8 +2212,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Error disallowing deletion</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" ht="29.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="K50" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Error disallowing deletion' }</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>34</v>
       </c>
@@ -1992,8 +2237,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0007] Delete by user with allowance manually created whse. shpt. line</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K51" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0007 'Delete by user with allowance manually created whse. shpt. line' {</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>34</v>
       </c>
@@ -2016,8 +2265,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K52" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Disable "Unblock Deletion of Shpt. Line" on warehouse setup'</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>34</v>
       </c>
@@ -2040,8 +2293,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Location with require shipment</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K53" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Location with require shipment'</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>34</v>
       </c>
@@ -2064,8 +2321,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K54" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user with allowance'</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>34</v>
       </c>
@@ -2088,8 +2349,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Manually created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K55" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Manually created warehouse shipment from released sales order with one line with require shipment location'</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>34</v>
       </c>
@@ -2112,8 +2377,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] Delete warehouse shipment line</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K56" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Delete warehouse shipment line'</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>34</v>
       </c>
@@ -2136,8 +2405,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" ht="29.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="K57" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Warehouse shipment line is deleted' }</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>34</v>
       </c>
@@ -2159,8 +2432,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0008] Delete  by user with allowance automatically created whse. shpt. Line with confirmation</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K58" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0008 'Delete  by user with allowance automatically created whse. shpt. Line with confirmation' {</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>34</v>
       </c>
@@ -2185,8 +2462,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K59" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Disable "Unblock Deletion of Shpt. Line" on warehouse setup'</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>34</v>
       </c>
@@ -2211,8 +2492,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Location with require shipment</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K60" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Location with require shipment'</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>34</v>
       </c>
@@ -2237,8 +2522,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K61" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user with allowance'</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>34</v>
       </c>
@@ -2263,8 +2552,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K62" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Automatically created warehouse shipment from released sales order with one line with require shipment location'</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>34</v>
       </c>
@@ -2289,8 +2582,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] Delete warehouse shipment line and select yes in confirmation</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K63" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Delete warehouse shipment line and select yes in confirmation'</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>34</v>
       </c>
@@ -2315,8 +2612,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Warehouse shipment line is deleted</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" ht="30.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="K64" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Warehouse shipment line is deleted' }</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>34</v>
       </c>
@@ -2338,8 +2639,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0011] Delete by user with allowance automatically created whse. shpt. line with no confirmation</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K65" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0011 'Delete by user with allowance automatically created whse. shpt. line with no confirmation' {</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>34</v>
       </c>
@@ -2364,8 +2669,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Enable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K66" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Enable "Unblock Deletion of Shpt. Line" on warehouse setup'</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>34</v>
       </c>
@@ -2390,8 +2699,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Location with require shipment</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K67" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Location with require shipment'</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>34</v>
       </c>
@@ -2416,8 +2729,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Warehouse employee for current user with allowance</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K68" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user with allowance'</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>34</v>
       </c>
@@ -2442,8 +2759,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Automatically created warehouse shipment from released sales order with one line with require shipment location</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K69" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Automatically created warehouse shipment from released sales order with one line with require shipment location'</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>34</v>
       </c>
@@ -2468,8 +2789,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] Delete warehouse shipment line and select no in confirm</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K70" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Delete warehouse shipment line and select no in confirm'</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>34</v>
       </c>
@@ -2494,8 +2819,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Empty error occurred</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" ht="29.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="K71" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Empty error occurred' }</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>34</v>
       </c>
@@ -2517,8 +2846,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0010] "Allowed to Delete Shpt. Line" is not editable on warehouse employees page</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K72" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0010 '"Allowed to Delete Shpt. Line" is not editable on warehouse employees page' {</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>34</v>
       </c>
@@ -2543,8 +2876,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Location</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K73" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Location'</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>34</v>
       </c>
@@ -2569,8 +2906,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Warehouse employee for current user</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K74" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse employee for current user'</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>34</v>
       </c>
@@ -2595,8 +2936,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] Disable "Unblock Deletion of Shpt. Line" on warehouse setup</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K75" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Disable "Unblock Deletion of Shpt. Line" on warehouse setup'</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>34</v>
       </c>
@@ -2621,11 +2966,14 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Allowed to Delete Shpt. Line is not editable on warehouse employees page</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" collapsed="1" x14ac:dyDescent="0.25"/>
+      <c r="K76" s="13" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Allowed to Delete Shpt. Line is not editable on warehouse employees page' } }</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="colorScale" priority="30">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2637,47 +2985,47 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="disabled">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="disabled">
       <formula>NOT(ISERROR(SEARCH("disabled",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="enabled">
+    <cfRule type="containsText" dxfId="5" priority="11" operator="containsText" text="enabled">
       <formula>NOT(ISERROR(SEARCH("enabled",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F65:F71">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:D71">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Solved failing tests #7
</commit_message>
<xml_diff>
--- a/VSCode/Blocking Deletion of Warehouse Shipment Lines/Test/atdd.scenarios/ATDD Scenarios - Blocking Deletion of Warehouse Shipment Lines.xlsx
+++ b/VSCode/Blocking Deletion of Warehouse Shipment Lines/Test/atdd.scenarios/ATDD Scenarios - Blocking Deletion of Warehouse Shipment Lines.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc van Vugt\source\repos\Test-Automation-Examples\VSCode\Blocking Deletion of Warehouse Shipment Lines\Test\atdd.scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2a63c87061b9b9b/Training/Test Automation/Online Course/9. January 2021/Session 4/Demo/Blocking Deletion/Test - ATDD.TestScriptor/atdd.scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C20E0EB-2CA4-4C30-84E8-617F516B14A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{1C20E0EB-2CA4-4C30-84E8-617F516B14A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EFE978A1-810B-4E97-AF23-0EE0B939A1CA}"/>
   <bookViews>
-    <workbookView xWindow="29610" yWindow="180" windowWidth="24510" windowHeight="15990" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="47">
   <si>
     <t>Feature</t>
   </si>
@@ -166,6 +169,12 @@
   </si>
   <si>
     <t>ATDD.TestScriptor Format</t>
+  </si>
+  <si>
+    <t>Allowed to Delete Shpt. Line is editable on warehouse employees page</t>
+  </si>
+  <si>
+    <t>"Allowed to Delete Shpt. Line" is editable on warehouse employees page</t>
   </si>
 </sst>
 </file>
@@ -298,6 +307,9 @@
   </cellStyles>
   <dxfs count="23">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -317,6 +329,51 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -410,54 +467,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -472,27 +481,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:L76" totalsRowShown="0" headerRowDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:L76" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A1:L76" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{8363E7FF-10AC-4A2B-AF58-2B6F4A3A2982}" name="Feature" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{47ED26B9-CBC1-4AA1-A3A9-843BF13AA89B}" name="Sub Feature" dataDxfId="20"/>
-    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{FC90C2DF-011C-4E76-8C03-6E75B2478287}" name="Positive-negative" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{8363E7FF-10AC-4A2B-AF58-2B6F4A3A2982}" name="Feature" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{47ED26B9-CBC1-4AA1-A3A9-843BF13AA89B}" name="Sub Feature" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{FC90C2DF-011C-4E76-8C03-6E75B2478287}" name="Positive-negative" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{824F4994-529B-42E7-960A-C52362C8177D}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="14">
+    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="3">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="13">
+    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{C88A1207-6598-4461-BC21-DEF845DAC115}" name="ATDD.TestScriptor Format" dataDxfId="0">
+    <tableColumn id="12" xr3:uid="{C88A1207-6598-4461-BC21-DEF845DAC115}" name="ATDD.TestScriptor Format" dataDxfId="1">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -797,9 +806,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B1ED69-5F96-4A81-993F-0E906F475813}">
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="8" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G4" sqref="G4"/>
+      <selection pane="topRight" activeCell="K36" sqref="K36:K76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2833,22 +2842,22 @@
       </c>
       <c r="D72" s="10"/>
       <c r="E72" s="3" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="H72" s="5">
         <v>10</v>
       </c>
       <c r="I72" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0010] "Allowed to Delete Shpt. Line" is not editable on warehouse employees page</v>
+        <v>[SCENARIO #0010] "Allowed to Delete Shpt. Line" is editable on warehouse employees page</v>
       </c>
       <c r="J72" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0010] "Allowed to Delete Shpt. Line" is not editable on warehouse employees page</v>
+        <v>//[SCENARIO #0010] "Allowed to Delete Shpt. Line" is editable on warehouse employees page</v>
       </c>
       <c r="K72" s="13" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0010 '"Allowed to Delete Shpt. Line" is not editable on warehouse employees page' {</v>
+        <v>Scenario 0010 '"Allowed to Delete Shpt. Line" is editable on warehouse employees page' {</v>
       </c>
     </row>
     <row r="73" spans="1:11" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2953,22 +2962,22 @@
         <v>20</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="H76" s="5">
         <v>10</v>
       </c>
       <c r="I76" s="6" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]],"/",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Allowed to Delete Shpt. Line is not editable on warehouse employees page</v>
+        <v>[THEN] Allowed to Delete Shpt. Line is editable on warehouse employees page</v>
       </c>
       <c r="J76" s="7" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Allowed to Delete Shpt. Line is not editable on warehouse employees page</v>
+        <v>//[THEN] Allowed to Delete Shpt. Line is editable on warehouse employees page</v>
       </c>
       <c r="K76" s="13" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Allowed to Delete Shpt. Line is not editable on warehouse employees page' } }</v>
+        <v>Then 'Allowed to Delete Shpt. Line is editable on warehouse employees page' } }</v>
       </c>
     </row>
   </sheetData>
@@ -2985,47 +2994,47 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="disabled">
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="disabled">
       <formula>NOT(ISERROR(SEARCH("disabled",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="11" operator="containsText" text="enabled">
+    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="enabled">
       <formula>NOT(ISERROR(SEARCH("enabled",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F65:F71">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:D71">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>